<commit_message>
Updated Financial Statements ✅ + Updated Index page for Contacts ✅
</commit_message>
<xml_diff>
--- a/Financial Projections.xlsx
+++ b/Financial Projections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hadir\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hadir\Documents\Business things\Prime-Properties\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1927CC5-AF69-4063-8702-F01E769918D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E321D4E7-6238-47EB-9889-8862585B3AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed Profit &amp; Loss" sheetId="3" r:id="rId1"/>
@@ -32,16 +32,8 @@
     <definedName name="Type">'[3]Maintenance Work Order'!#REF!</definedName>
     <definedName name="valHighlight">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -2493,9 +2485,9 @@
   </sheetPr>
   <dimension ref="A1:S137"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B137" sqref="B137:J137"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2590,72 +2582,60 @@
         <v>31</v>
       </c>
       <c r="C6" s="107">
-        <f>C34</f>
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="D6" s="107">
-        <f t="shared" ref="D6" si="0">D34</f>
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="E6" s="107">
-        <f>E34</f>
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="F6" s="104">
         <f>SUM(C6:E6)</f>
-        <v>0</v>
+        <v>180000</v>
       </c>
       <c r="G6" s="130">
-        <f>G34</f>
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="H6" s="130">
-        <f t="shared" ref="H6:I6" si="1">H34</f>
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="I6" s="130">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>95000</v>
       </c>
       <c r="J6" s="145">
         <f>SUM(G6:I6)</f>
-        <v>0</v>
+        <v>265000</v>
       </c>
       <c r="K6" s="139">
-        <f>K34</f>
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="L6" s="139">
-        <f>L34</f>
-        <v>0</v>
+        <v>105000</v>
       </c>
       <c r="M6" s="139">
-        <f>M34</f>
-        <v>0</v>
+        <v>110000</v>
       </c>
       <c r="N6" s="149">
         <f>SUM(K6:M6)</f>
-        <v>0</v>
+        <v>315000</v>
       </c>
       <c r="O6" s="157">
-        <f>O34</f>
-        <v>0</v>
+        <v>115000</v>
       </c>
       <c r="P6" s="157">
-        <f t="shared" ref="P6:Q6" si="2">P34</f>
-        <v>0</v>
+        <v>120000</v>
       </c>
       <c r="Q6" s="157">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>125000</v>
       </c>
       <c r="R6" s="171">
         <f>SUM(O6:Q6)</f>
-        <v>0</v>
+        <v>360000</v>
       </c>
       <c r="S6" s="184">
         <f>SUM(F6,J6,N6,R6)</f>
-        <v>0</v>
+        <v>1120000</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2663,72 +2643,60 @@
         <v>77</v>
       </c>
       <c r="C7" s="108">
-        <f>C135</f>
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="D7" s="108">
-        <f>D135</f>
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="E7" s="108">
-        <f>E135</f>
-        <v>0</v>
+        <v>45000</v>
       </c>
       <c r="F7" s="105">
         <f>SUM(C7:E7)</f>
-        <v>0</v>
+        <v>120000</v>
       </c>
       <c r="G7" s="131">
-        <f>G135</f>
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="H7" s="131">
-        <f>H135</f>
-        <v>0</v>
+        <v>55000</v>
       </c>
       <c r="I7" s="131">
-        <f>I135</f>
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="J7" s="146">
         <f>SUM(G7:I7)</f>
-        <v>0</v>
+        <v>165000</v>
       </c>
       <c r="K7" s="140">
-        <f>K135</f>
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="L7" s="140">
-        <f>L135</f>
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="M7" s="140">
-        <f>M135</f>
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="N7" s="150">
         <f>SUM(K7:M7)</f>
-        <v>0</v>
+        <v>215000</v>
       </c>
       <c r="O7" s="158">
-        <f>O135</f>
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="P7" s="158">
-        <f>P135</f>
-        <v>0</v>
+        <v>85000</v>
       </c>
       <c r="Q7" s="158">
-        <f>Q135</f>
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="R7" s="172">
         <f>SUM(O7:Q7)</f>
-        <v>0</v>
+        <v>255000</v>
       </c>
       <c r="S7" s="185">
         <f>SUM(F7,J7,N7,R7)</f>
-        <v>0</v>
+        <v>755000</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2736,72 +2704,71 @@
         <v>132</v>
       </c>
       <c r="C8" s="102">
-        <f>C6-C7</f>
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="D8" s="102">
-        <f t="shared" ref="D8:E8" si="3">D6-D7</f>
-        <v>0</v>
+        <f t="shared" ref="D8:E8" si="0">D6-D7</f>
+        <v>20000</v>
       </c>
       <c r="E8" s="102">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>25000</v>
       </c>
       <c r="F8" s="101">
         <f>SUM(C8:E8)</f>
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="G8" s="144">
         <f>G6-G7</f>
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="H8" s="144">
-        <f t="shared" ref="H8" si="4">H6-H7</f>
-        <v>0</v>
+        <f t="shared" ref="H8" si="1">H6-H7</f>
+        <v>35000</v>
       </c>
       <c r="I8" s="144">
-        <f t="shared" ref="I8" si="5">I6-I7</f>
-        <v>0</v>
+        <f t="shared" ref="I8" si="2">I6-I7</f>
+        <v>35000</v>
       </c>
       <c r="J8" s="143">
         <f>SUM(G8:I8)</f>
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="K8" s="147">
         <f>K6-K7</f>
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="L8" s="147">
-        <f t="shared" ref="L8" si="6">L6-L7</f>
-        <v>0</v>
+        <f t="shared" ref="L8" si="3">L6-L7</f>
+        <v>35000</v>
       </c>
       <c r="M8" s="147">
-        <f t="shared" ref="M8" si="7">M6-M7</f>
-        <v>0</v>
+        <f t="shared" ref="M8" si="4">M6-M7</f>
+        <v>30000</v>
       </c>
       <c r="N8" s="153">
         <f>SUM(K8:M8)</f>
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="O8" s="169">
         <f>O6-O7</f>
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="P8" s="169">
-        <f t="shared" ref="P8" si="8">P6-P7</f>
-        <v>0</v>
+        <f t="shared" ref="P8" si="5">P6-P7</f>
+        <v>35000</v>
       </c>
       <c r="Q8" s="169">
-        <f t="shared" ref="Q8" si="9">Q6-Q7</f>
-        <v>0</v>
+        <f t="shared" ref="Q8" si="6">Q6-Q7</f>
+        <v>35000</v>
       </c>
       <c r="R8" s="175">
         <f>SUM(O8:Q8)</f>
-        <v>0</v>
+        <v>105000</v>
       </c>
       <c r="S8" s="186">
         <f>SUM(F8,J8,N8,R8)</f>
-        <v>0</v>
+        <v>365000</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2810,54 +2777,54 @@
       </c>
       <c r="C9" s="100">
         <f>C8</f>
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="D9" s="100">
         <f>C9+D8</f>
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="E9" s="100">
         <f>D9+E8</f>
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="F9" s="99"/>
       <c r="G9" s="141">
         <f>E9+G8</f>
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="H9" s="141">
         <f>G9+H8</f>
-        <v>0</v>
+        <v>125000</v>
       </c>
       <c r="I9" s="141">
         <f>H9+I8</f>
-        <v>0</v>
+        <v>160000</v>
       </c>
       <c r="J9" s="142"/>
       <c r="K9" s="152">
         <f>I9+K8</f>
-        <v>0</v>
+        <v>195000</v>
       </c>
       <c r="L9" s="152">
         <f>K9+L8</f>
-        <v>0</v>
+        <v>230000</v>
       </c>
       <c r="M9" s="152">
         <f>L9+M8</f>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="N9" s="154"/>
       <c r="O9" s="173">
         <f>M9+O8</f>
-        <v>0</v>
+        <v>295000</v>
       </c>
       <c r="P9" s="173">
         <f>O9+P8</f>
-        <v>0</v>
+        <v>330000</v>
       </c>
       <c r="Q9" s="173">
         <f>P9+Q8</f>
-        <v>0</v>
+        <v>365000</v>
       </c>
       <c r="R9" s="174"/>
     </row>
@@ -2921,11 +2888,11 @@
         <v/>
       </c>
       <c r="D12" s="193" t="str">
-        <f t="shared" ref="D12:E12" si="10">IFERROR(D6/D27,"")</f>
+        <f t="shared" ref="D12:E12" si="7">IFERROR(D6/D27,"")</f>
         <v/>
       </c>
       <c r="E12" s="193" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F12" s="201"/>
@@ -2934,11 +2901,11 @@
         <v/>
       </c>
       <c r="H12" s="194" t="str">
-        <f t="shared" ref="H12:I12" si="11">IFERROR(H6/H27,"")</f>
+        <f t="shared" ref="H12:I12" si="8">IFERROR(H6/H27,"")</f>
         <v/>
       </c>
       <c r="I12" s="194" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J12" s="202"/>
@@ -2947,11 +2914,11 @@
         <v/>
       </c>
       <c r="L12" s="195" t="str">
-        <f t="shared" ref="L12:M12" si="12">IFERROR(L6/L27,"")</f>
+        <f t="shared" ref="L12:M12" si="9">IFERROR(L6/L27,"")</f>
         <v/>
       </c>
       <c r="M12" s="195" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="N12" s="203"/>
@@ -2960,11 +2927,11 @@
         <v/>
       </c>
       <c r="P12" s="196" t="str">
-        <f t="shared" ref="P12:Q12" si="13">IFERROR(P6/P27,"")</f>
+        <f t="shared" ref="P12:Q12" si="10">IFERROR(P6/P27,"")</f>
         <v/>
       </c>
       <c r="Q12" s="196" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="R12" s="204"/>
@@ -2978,11 +2945,11 @@
         <v/>
       </c>
       <c r="D13" s="193" t="str">
-        <f t="shared" ref="D13:E13" si="14">IFERROR(D8/D27,"")</f>
+        <f t="shared" ref="D13:E13" si="11">IFERROR(D8/D27,"")</f>
         <v/>
       </c>
       <c r="E13" s="193" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="F13" s="201"/>
@@ -2991,11 +2958,11 @@
         <v/>
       </c>
       <c r="H13" s="194" t="str">
-        <f t="shared" ref="H13:I13" si="15">IFERROR(H8/H27,"")</f>
+        <f t="shared" ref="H13:I13" si="12">IFERROR(H8/H27,"")</f>
         <v/>
       </c>
       <c r="I13" s="194" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="J13" s="202"/>
@@ -3004,11 +2971,11 @@
         <v/>
       </c>
       <c r="L13" s="195" t="str">
-        <f t="shared" ref="L13:M13" si="16">IFERROR(L8/L27,"")</f>
+        <f t="shared" ref="L13:M13" si="13">IFERROR(L8/L27,"")</f>
         <v/>
       </c>
       <c r="M13" s="195" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N13" s="203"/>
@@ -3017,11 +2984,11 @@
         <v/>
       </c>
       <c r="P13" s="196" t="str">
-        <f t="shared" ref="P13:Q13" si="17">IFERROR(P8/P27,"")</f>
+        <f t="shared" ref="P13:Q13" si="14">IFERROR(P8/P27,"")</f>
         <v/>
       </c>
       <c r="Q13" s="196" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="R13" s="204"/>
@@ -3035,11 +3002,11 @@
         <v/>
       </c>
       <c r="D14" s="128" t="str">
-        <f t="shared" ref="D14:E14" si="18">IFERROR(D6/D33,"")</f>
+        <f t="shared" ref="D14:E14" si="15">IFERROR(D6/D33,"")</f>
         <v/>
       </c>
       <c r="E14" s="128" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="F14" s="201"/>
@@ -3048,11 +3015,11 @@
         <v/>
       </c>
       <c r="H14" s="129" t="str">
-        <f t="shared" ref="H14:I14" si="19">IFERROR(H6/H33,"")</f>
+        <f t="shared" ref="H14:I14" si="16">IFERROR(H6/H33,"")</f>
         <v/>
       </c>
       <c r="I14" s="129" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="J14" s="202"/>
@@ -3061,11 +3028,11 @@
         <v/>
       </c>
       <c r="L14" s="138" t="str">
-        <f t="shared" ref="L14:M14" si="20">IFERROR(L6/L33,"")</f>
+        <f t="shared" ref="L14:M14" si="17">IFERROR(L6/L33,"")</f>
         <v/>
       </c>
       <c r="M14" s="138" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="N14" s="203"/>
@@ -3074,11 +3041,11 @@
         <v/>
       </c>
       <c r="P14" s="161" t="str">
-        <f t="shared" ref="P14:Q14" si="21">IFERROR(P6/P33,"")</f>
+        <f t="shared" ref="P14:Q14" si="18">IFERROR(P6/P33,"")</f>
         <v/>
       </c>
       <c r="Q14" s="161" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="R14" s="204"/>
@@ -3092,11 +3059,11 @@
         <v/>
       </c>
       <c r="D15" s="126" t="str">
-        <f t="shared" ref="D15:E15" si="22">IFERROR((D7/(1-D33/D27)),"")</f>
+        <f t="shared" ref="D15:E15" si="19">IFERROR((D7/(1-D33/D27)),"")</f>
         <v/>
       </c>
       <c r="E15" s="126" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="F15" s="201"/>
@@ -3105,11 +3072,11 @@
         <v/>
       </c>
       <c r="H15" s="127" t="str">
-        <f t="shared" ref="H15:I15" si="23">IFERROR((H7/(1-H33/H27)),"")</f>
+        <f t="shared" ref="H15:I15" si="20">IFERROR((H7/(1-H33/H27)),"")</f>
         <v/>
       </c>
       <c r="I15" s="127" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="J15" s="202"/>
@@ -3118,11 +3085,11 @@
         <v/>
       </c>
       <c r="L15" s="137" t="str">
-        <f t="shared" ref="L15:M15" si="24">IFERROR((L7/(1-L33/L27)),"")</f>
+        <f t="shared" ref="L15:M15" si="21">IFERROR((L7/(1-L33/L27)),"")</f>
         <v/>
       </c>
       <c r="M15" s="137" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="N15" s="203"/>
@@ -3131,11 +3098,11 @@
         <v/>
       </c>
       <c r="P15" s="160" t="str">
-        <f t="shared" ref="P15:Q15" si="25">IFERROR((P7/(1-P33/P27)),"")</f>
+        <f t="shared" ref="P15:Q15" si="22">IFERROR((P7/(1-P33/P27)),"")</f>
         <v/>
       </c>
       <c r="Q15" s="160" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="R15" s="204"/>
@@ -3293,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="12">
-        <f t="shared" ref="S20:S22" si="26">SUM(F20,J20,N20,R20)</f>
+        <f t="shared" ref="S20:S22" si="23">SUM(F20,J20,N20,R20)</f>
         <v>0</v>
       </c>
     </row>
@@ -3330,7 +3297,7 @@
         <v>0</v>
       </c>
       <c r="S21" s="12">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -3343,15 +3310,15 @@
         <v>0</v>
       </c>
       <c r="D22" s="29">
-        <f t="shared" ref="D22:F22" si="27">SUM(D19:D21)</f>
+        <f t="shared" ref="D22:F22" si="24">SUM(D19:D21)</f>
         <v>0</v>
       </c>
       <c r="E22" s="29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="F22" s="35">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="G22" s="29">
@@ -3359,15 +3326,15 @@
         <v>0</v>
       </c>
       <c r="H22" s="29">
-        <f t="shared" ref="H22" si="28">SUM(H19:H21)</f>
+        <f t="shared" ref="H22" si="25">SUM(H19:H21)</f>
         <v>0</v>
       </c>
       <c r="I22" s="29">
-        <f t="shared" ref="I22" si="29">SUM(I19:I21)</f>
+        <f t="shared" ref="I22" si="26">SUM(I19:I21)</f>
         <v>0</v>
       </c>
       <c r="J22" s="37">
-        <f t="shared" ref="J22" si="30">SUM(J19:J21)</f>
+        <f t="shared" ref="J22" si="27">SUM(J19:J21)</f>
         <v>0</v>
       </c>
       <c r="K22" s="29">
@@ -3375,15 +3342,15 @@
         <v>0</v>
       </c>
       <c r="L22" s="29">
-        <f t="shared" ref="L22" si="31">SUM(L19:L21)</f>
+        <f t="shared" ref="L22" si="28">SUM(L19:L21)</f>
         <v>0</v>
       </c>
       <c r="M22" s="29">
-        <f t="shared" ref="M22" si="32">SUM(M19:M21)</f>
+        <f t="shared" ref="M22" si="29">SUM(M19:M21)</f>
         <v>0</v>
       </c>
       <c r="N22" s="37">
-        <f t="shared" ref="N22" si="33">SUM(N19:N21)</f>
+        <f t="shared" ref="N22" si="30">SUM(N19:N21)</f>
         <v>0</v>
       </c>
       <c r="O22" s="29">
@@ -3391,19 +3358,19 @@
         <v>0</v>
       </c>
       <c r="P22" s="29">
-        <f t="shared" ref="P22" si="34">SUM(P19:P21)</f>
+        <f t="shared" ref="P22" si="31">SUM(P19:P21)</f>
         <v>0</v>
       </c>
       <c r="Q22" s="29">
-        <f t="shared" ref="Q22" si="35">SUM(Q19:Q21)</f>
+        <f t="shared" ref="Q22" si="32">SUM(Q19:Q21)</f>
         <v>0</v>
       </c>
       <c r="R22" s="37">
-        <f t="shared" ref="R22" si="36">SUM(R19:R21)</f>
+        <f t="shared" ref="R22" si="33">SUM(R19:R21)</f>
         <v>0</v>
       </c>
       <c r="S22" s="38">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -3499,7 +3466,7 @@
         <v>0</v>
       </c>
       <c r="S25" s="12">
-        <f t="shared" ref="S25" si="37">SUM(F25,J25,N25,R25)</f>
+        <f t="shared" ref="S25" si="34">SUM(F25,J25,N25,R25)</f>
         <v>0</v>
       </c>
     </row>
@@ -3512,11 +3479,11 @@
         <v>0</v>
       </c>
       <c r="D26" s="10">
-        <f t="shared" ref="D26:E26" si="38">SUM(D24:D25)</f>
+        <f t="shared" ref="D26:E26" si="35">SUM(D24:D25)</f>
         <v>0</v>
       </c>
       <c r="E26" s="10">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="F26" s="110">
@@ -3528,11 +3495,11 @@
         <v>0</v>
       </c>
       <c r="H26" s="10">
-        <f t="shared" ref="H26" si="39">SUM(H24:H25)</f>
+        <f t="shared" ref="H26" si="36">SUM(H24:H25)</f>
         <v>0</v>
       </c>
       <c r="I26" s="10">
-        <f t="shared" ref="I26" si="40">SUM(I24:I25)</f>
+        <f t="shared" ref="I26" si="37">SUM(I24:I25)</f>
         <v>0</v>
       </c>
       <c r="J26" s="20">
@@ -3544,11 +3511,11 @@
         <v>0</v>
       </c>
       <c r="L26" s="10">
-        <f t="shared" ref="L26" si="41">SUM(L24:L25)</f>
+        <f t="shared" ref="L26" si="38">SUM(L24:L25)</f>
         <v>0</v>
       </c>
       <c r="M26" s="10">
-        <f t="shared" ref="M26" si="42">SUM(M24:M25)</f>
+        <f t="shared" ref="M26" si="39">SUM(M24:M25)</f>
         <v>0</v>
       </c>
       <c r="N26" s="16">
@@ -3560,11 +3527,11 @@
         <v>0</v>
       </c>
       <c r="P26" s="10">
-        <f t="shared" ref="P26" si="43">SUM(P24:P25)</f>
+        <f t="shared" ref="P26" si="40">SUM(P24:P25)</f>
         <v>0</v>
       </c>
       <c r="Q26" s="10">
-        <f t="shared" ref="Q26" si="44">SUM(Q24:Q25)</f>
+        <f t="shared" ref="Q26" si="41">SUM(Q24:Q25)</f>
         <v>0</v>
       </c>
       <c r="R26" s="178">
@@ -3585,15 +3552,15 @@
         <v>0</v>
       </c>
       <c r="D27" s="33">
-        <f t="shared" ref="D27:F27" si="45">D22-D26</f>
+        <f t="shared" ref="D27:F27" si="42">D22-D26</f>
         <v>0</v>
       </c>
       <c r="E27" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="F27" s="31">
-        <f t="shared" si="45"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G27" s="34">
@@ -3601,15 +3568,15 @@
         <v>0</v>
       </c>
       <c r="H27" s="33">
-        <f t="shared" ref="H27" si="46">H22-H26</f>
+        <f t="shared" ref="H27" si="43">H22-H26</f>
         <v>0</v>
       </c>
       <c r="I27" s="33">
-        <f t="shared" ref="I27" si="47">I22-I26</f>
+        <f t="shared" ref="I27" si="44">I22-I26</f>
         <v>0</v>
       </c>
       <c r="J27" s="32">
-        <f t="shared" ref="J27" si="48">J22-J26</f>
+        <f t="shared" ref="J27" si="45">J22-J26</f>
         <v>0</v>
       </c>
       <c r="K27" s="34">
@@ -3617,15 +3584,15 @@
         <v>0</v>
       </c>
       <c r="L27" s="33">
-        <f t="shared" ref="L27" si="49">L22-L26</f>
+        <f t="shared" ref="L27" si="46">L22-L26</f>
         <v>0</v>
       </c>
       <c r="M27" s="33">
-        <f t="shared" ref="M27" si="50">M22-M26</f>
+        <f t="shared" ref="M27" si="47">M22-M26</f>
         <v>0</v>
       </c>
       <c r="N27" s="32">
-        <f t="shared" ref="N27" si="51">N22-N26</f>
+        <f t="shared" ref="N27" si="48">N22-N26</f>
         <v>0</v>
       </c>
       <c r="O27" s="34">
@@ -3633,15 +3600,15 @@
         <v>0</v>
       </c>
       <c r="P27" s="33">
-        <f t="shared" ref="P27" si="52">P22-P26</f>
+        <f t="shared" ref="P27" si="49">P22-P26</f>
         <v>0</v>
       </c>
       <c r="Q27" s="33">
-        <f t="shared" ref="Q27" si="53">Q22-Q26</f>
+        <f t="shared" ref="Q27" si="50">Q22-Q26</f>
         <v>0</v>
       </c>
       <c r="R27" s="32">
-        <f t="shared" ref="R27" si="54">R22-R26</f>
+        <f t="shared" ref="R27" si="51">R22-R26</f>
         <v>0</v>
       </c>
       <c r="S27" s="38">
@@ -3741,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="S30" s="12">
-        <f t="shared" ref="S30:S32" si="55">SUM(F30,J30,N30,R30)</f>
+        <f t="shared" ref="S30:S32" si="52">SUM(F30,J30,N30,R30)</f>
         <v>0</v>
       </c>
     </row>
@@ -3754,11 +3721,11 @@
         <v>0</v>
       </c>
       <c r="D31" s="10">
-        <f t="shared" ref="D31:E31" si="56">SUM(D29:D30)</f>
+        <f t="shared" ref="D31:E31" si="53">SUM(D29:D30)</f>
         <v>0</v>
       </c>
       <c r="E31" s="10">
-        <f t="shared" si="56"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="F31" s="36">
@@ -3770,11 +3737,11 @@
         <v>0</v>
       </c>
       <c r="H31" s="10">
-        <f t="shared" ref="H31:I31" si="57">SUM(H29:H30)</f>
+        <f t="shared" ref="H31:I31" si="54">SUM(H29:H30)</f>
         <v>0</v>
       </c>
       <c r="I31" s="10">
-        <f t="shared" si="57"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="J31" s="36">
@@ -3786,11 +3753,11 @@
         <v>0</v>
       </c>
       <c r="L31" s="10">
-        <f t="shared" ref="L31:M31" si="58">SUM(L29:L30)</f>
+        <f t="shared" ref="L31:M31" si="55">SUM(L29:L30)</f>
         <v>0</v>
       </c>
       <c r="M31" s="10">
-        <f t="shared" si="58"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="N31" s="36">
@@ -3802,11 +3769,11 @@
         <v>0</v>
       </c>
       <c r="P31" s="10">
-        <f t="shared" ref="P31:Q31" si="59">SUM(P29:P30)</f>
+        <f t="shared" ref="P31:Q31" si="56">SUM(P29:P30)</f>
         <v>0</v>
       </c>
       <c r="Q31" s="10">
-        <f t="shared" si="59"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="R31" s="36">
@@ -3851,7 +3818,7 @@
         <v>0</v>
       </c>
       <c r="S32" s="12">
-        <f t="shared" si="55"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
     </row>
@@ -3864,59 +3831,59 @@
         <v>0</v>
       </c>
       <c r="D33" s="33">
-        <f t="shared" ref="D33:Q33" si="60">D31-D32</f>
+        <f t="shared" ref="D33:Q33" si="57">D31-D32</f>
         <v>0</v>
       </c>
       <c r="E33" s="33">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="F33" s="32">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="G33" s="34">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="H33" s="33">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="I33" s="33">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="J33" s="32">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="K33" s="34">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="L33" s="33">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="M33" s="33">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="N33" s="32">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="O33" s="34">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="P33" s="33">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="Q33" s="33">
-        <f t="shared" si="60"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="R33" s="32">
@@ -3937,11 +3904,11 @@
         <v>0</v>
       </c>
       <c r="D34" s="115">
-        <f t="shared" ref="D34:E34" si="61">D27-D33</f>
+        <f t="shared" ref="D34:E34" si="58">D27-D33</f>
         <v>0</v>
       </c>
       <c r="E34" s="115">
-        <f t="shared" si="61"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="F34" s="114">
@@ -3953,11 +3920,11 @@
         <v>0</v>
       </c>
       <c r="H34" s="119">
-        <f t="shared" ref="H34" si="62">H27-H33</f>
+        <f t="shared" ref="H34" si="59">H27-H33</f>
         <v>0</v>
       </c>
       <c r="I34" s="119">
-        <f t="shared" ref="I34" si="63">I27-I33</f>
+        <f t="shared" ref="I34" si="60">I27-I33</f>
         <v>0</v>
       </c>
       <c r="J34" s="120">
@@ -3969,11 +3936,11 @@
         <v>0</v>
       </c>
       <c r="L34" s="133">
-        <f t="shared" ref="L34" si="64">L27-L33</f>
+        <f t="shared" ref="L34" si="61">L27-L33</f>
         <v>0</v>
       </c>
       <c r="M34" s="133">
-        <f t="shared" ref="M34" si="65">M27-M33</f>
+        <f t="shared" ref="M34" si="62">M27-M33</f>
         <v>0</v>
       </c>
       <c r="N34" s="151">
@@ -3985,11 +3952,11 @@
         <v>0</v>
       </c>
       <c r="P34" s="163">
-        <f t="shared" ref="P34" si="66">P27-P33</f>
+        <f t="shared" ref="P34" si="63">P27-P33</f>
         <v>0</v>
       </c>
       <c r="Q34" s="163">
-        <f t="shared" ref="Q34" si="67">Q27-Q33</f>
+        <f t="shared" ref="Q34" si="64">Q27-Q33</f>
         <v>0</v>
       </c>
       <c r="R34" s="179">
@@ -4087,28 +4054,28 @@
       <c r="D38" s="113"/>
       <c r="E38" s="113"/>
       <c r="F38" s="110">
-        <f t="shared" ref="F38:F46" si="68">SUM(C38:E38)</f>
+        <f t="shared" ref="F38:F46" si="65">SUM(C38:E38)</f>
         <v>0</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="20">
-        <f t="shared" ref="J38:J46" si="69">SUM(G38:I38)</f>
+        <f t="shared" ref="J38:J46" si="66">SUM(G38:I38)</f>
         <v>0</v>
       </c>
       <c r="K38" s="18"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
       <c r="N38" s="16">
-        <f t="shared" ref="N38:N46" si="70">SUM(K38:M38)</f>
+        <f t="shared" ref="N38:N46" si="67">SUM(K38:M38)</f>
         <v>0</v>
       </c>
       <c r="O38" s="165"/>
       <c r="P38" s="166"/>
       <c r="Q38" s="166"/>
       <c r="R38" s="178">
-        <f t="shared" ref="R38:R46" si="71">SUM(O38:Q38)</f>
+        <f t="shared" ref="R38:R46" si="68">SUM(O38:Q38)</f>
         <v>0</v>
       </c>
       <c r="S38" s="12">
@@ -4124,32 +4091,32 @@
       <c r="D39" s="113"/>
       <c r="E39" s="113"/>
       <c r="F39" s="110">
-        <f t="shared" si="68"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
       <c r="J39" s="20">
-        <f t="shared" si="69"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="K39" s="18"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
       <c r="N39" s="16">
-        <f t="shared" si="70"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="O39" s="165"/>
       <c r="P39" s="166"/>
       <c r="Q39" s="166"/>
       <c r="R39" s="178">
-        <f t="shared" si="71"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="S39" s="12">
-        <f t="shared" ref="S39:S42" si="72">SUM(F39,J39,N39,R39)</f>
+        <f t="shared" ref="S39:S42" si="69">SUM(F39,J39,N39,R39)</f>
         <v>0</v>
       </c>
     </row>
@@ -4161,28 +4128,28 @@
       <c r="D40" s="113"/>
       <c r="E40" s="113"/>
       <c r="F40" s="110">
-        <f t="shared" si="68"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="20">
-        <f t="shared" si="69"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="K40" s="18"/>
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
       <c r="N40" s="16">
-        <f t="shared" si="70"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="O40" s="165"/>
       <c r="P40" s="166"/>
       <c r="Q40" s="166"/>
       <c r="R40" s="178">
-        <f t="shared" si="71"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="S40" s="12">
@@ -4198,32 +4165,32 @@
       <c r="D41" s="113"/>
       <c r="E41" s="113"/>
       <c r="F41" s="110">
-        <f t="shared" si="68"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="G41" s="22"/>
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
       <c r="J41" s="20">
-        <f t="shared" si="69"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="K41" s="18"/>
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
       <c r="N41" s="16">
-        <f t="shared" si="70"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="O41" s="165"/>
       <c r="P41" s="166"/>
       <c r="Q41" s="166"/>
       <c r="R41" s="178">
-        <f t="shared" si="71"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="S41" s="12">
-        <f t="shared" ref="S41" si="73">SUM(F41,J41,N41,R41)</f>
+        <f t="shared" ref="S41" si="70">SUM(F41,J41,N41,R41)</f>
         <v>0</v>
       </c>
     </row>
@@ -4235,32 +4202,32 @@
       <c r="D42" s="113"/>
       <c r="E42" s="113"/>
       <c r="F42" s="110">
-        <f t="shared" si="68"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="G42" s="22"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="J42" s="20">
-        <f t="shared" si="69"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="K42" s="18"/>
       <c r="L42" s="9"/>
       <c r="M42" s="9"/>
       <c r="N42" s="16">
-        <f t="shared" si="70"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="O42" s="165"/>
       <c r="P42" s="166"/>
       <c r="Q42" s="166"/>
       <c r="R42" s="178">
-        <f t="shared" si="71"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="S42" s="12">
-        <f t="shared" si="72"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
     </row>
@@ -4272,28 +4239,28 @@
       <c r="D43" s="113"/>
       <c r="E43" s="113"/>
       <c r="F43" s="110">
-        <f t="shared" si="68"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="J43" s="20">
-        <f t="shared" si="69"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="K43" s="18"/>
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
       <c r="N43" s="16">
-        <f t="shared" si="70"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="O43" s="165"/>
       <c r="P43" s="166"/>
       <c r="Q43" s="166"/>
       <c r="R43" s="178">
-        <f t="shared" si="71"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="S43" s="12">
@@ -4309,32 +4276,32 @@
       <c r="D44" s="113"/>
       <c r="E44" s="113"/>
       <c r="F44" s="110">
-        <f t="shared" si="68"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="20">
-        <f t="shared" si="69"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="K44" s="18"/>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
       <c r="N44" s="16">
-        <f t="shared" si="70"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="O44" s="165"/>
       <c r="P44" s="166"/>
       <c r="Q44" s="166"/>
       <c r="R44" s="178">
-        <f t="shared" si="71"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="S44" s="12">
-        <f t="shared" ref="S44" si="74">SUM(F44,J44,N44,R44)</f>
+        <f t="shared" ref="S44" si="71">SUM(F44,J44,N44,R44)</f>
         <v>0</v>
       </c>
     </row>
@@ -4346,28 +4313,28 @@
       <c r="D45" s="113"/>
       <c r="E45" s="113"/>
       <c r="F45" s="110">
-        <f t="shared" si="68"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="20">
-        <f t="shared" si="69"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="K45" s="18"/>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" s="16">
-        <f t="shared" si="70"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="O45" s="165"/>
       <c r="P45" s="166"/>
       <c r="Q45" s="166"/>
       <c r="R45" s="178">
-        <f t="shared" si="71"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="S45" s="12">
@@ -4388,11 +4355,11 @@
         <v>0</v>
       </c>
       <c r="E46" s="111">
-        <f t="shared" ref="E46" si="75">SUM(E38:E45)</f>
+        <f t="shared" ref="E46" si="72">SUM(E38:E45)</f>
         <v>0</v>
       </c>
       <c r="F46" s="110">
-        <f t="shared" si="68"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="G46" s="23">
@@ -4404,11 +4371,11 @@
         <v>0</v>
       </c>
       <c r="I46" s="24">
-        <f t="shared" ref="I46" si="76">SUM(I38:I45)</f>
+        <f t="shared" ref="I46" si="73">SUM(I38:I45)</f>
         <v>0</v>
       </c>
       <c r="J46" s="20">
-        <f t="shared" si="69"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="K46" s="25">
@@ -4420,11 +4387,11 @@
         <v>0</v>
       </c>
       <c r="M46" s="26">
-        <f t="shared" ref="M46" si="77">SUM(M38:M45)</f>
+        <f t="shared" ref="M46" si="74">SUM(M38:M45)</f>
         <v>0</v>
       </c>
       <c r="N46" s="16">
-        <f t="shared" si="70"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="O46" s="180">
@@ -4440,7 +4407,7 @@
         <v>0</v>
       </c>
       <c r="R46" s="178">
-        <f t="shared" si="71"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="S46" s="38">
@@ -4478,28 +4445,28 @@
       <c r="D48" s="113"/>
       <c r="E48" s="113"/>
       <c r="F48" s="110">
-        <f t="shared" ref="F48:F58" si="78">SUM(C48:E48)</f>
+        <f t="shared" ref="F48:F58" si="75">SUM(C48:E48)</f>
         <v>0</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
       <c r="J48" s="20">
-        <f t="shared" ref="J48:J58" si="79">SUM(G48:I48)</f>
+        <f t="shared" ref="J48:J58" si="76">SUM(G48:I48)</f>
         <v>0</v>
       </c>
       <c r="K48" s="18"/>
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
       <c r="N48" s="16">
-        <f t="shared" ref="N48:N58" si="80">SUM(K48:M48)</f>
+        <f t="shared" ref="N48:N58" si="77">SUM(K48:M48)</f>
         <v>0</v>
       </c>
       <c r="O48" s="165"/>
       <c r="P48" s="166"/>
       <c r="Q48" s="166"/>
       <c r="R48" s="178">
-        <f t="shared" ref="R48:R58" si="81">SUM(O48:Q48)</f>
+        <f t="shared" ref="R48:R58" si="78">SUM(O48:Q48)</f>
         <v>0</v>
       </c>
       <c r="S48" s="12">
@@ -4515,32 +4482,32 @@
       <c r="D49" s="113"/>
       <c r="E49" s="113"/>
       <c r="F49" s="110">
-        <f t="shared" si="78"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
       <c r="J49" s="20">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="K49" s="18"/>
       <c r="L49" s="9"/>
       <c r="M49" s="9"/>
       <c r="N49" s="16">
-        <f t="shared" si="80"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="O49" s="165"/>
       <c r="P49" s="166"/>
       <c r="Q49" s="166"/>
       <c r="R49" s="178">
-        <f t="shared" si="81"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="S49" s="12">
-        <f t="shared" ref="S49" si="82">SUM(F49,J49,N49,R49)</f>
+        <f t="shared" ref="S49" si="79">SUM(F49,J49,N49,R49)</f>
         <v>0</v>
       </c>
     </row>
@@ -4552,28 +4519,28 @@
       <c r="D50" s="113"/>
       <c r="E50" s="113"/>
       <c r="F50" s="110">
-        <f t="shared" si="78"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="J50" s="20">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="K50" s="18"/>
       <c r="L50" s="9"/>
       <c r="M50" s="9"/>
       <c r="N50" s="16">
-        <f t="shared" si="80"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="O50" s="165"/>
       <c r="P50" s="166"/>
       <c r="Q50" s="166"/>
       <c r="R50" s="178">
-        <f t="shared" si="81"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="S50" s="12">
@@ -4589,32 +4556,32 @@
       <c r="D51" s="113"/>
       <c r="E51" s="113"/>
       <c r="F51" s="110">
-        <f t="shared" si="78"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
       <c r="J51" s="20">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="K51" s="18"/>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
       <c r="N51" s="16">
-        <f t="shared" si="80"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="O51" s="165"/>
       <c r="P51" s="166"/>
       <c r="Q51" s="166"/>
       <c r="R51" s="178">
-        <f t="shared" si="81"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="S51" s="12">
-        <f t="shared" ref="S51:S52" si="83">SUM(F51,J51,N51,R51)</f>
+        <f t="shared" ref="S51:S52" si="80">SUM(F51,J51,N51,R51)</f>
         <v>0</v>
       </c>
     </row>
@@ -4626,32 +4593,32 @@
       <c r="D52" s="113"/>
       <c r="E52" s="113"/>
       <c r="F52" s="110">
-        <f t="shared" si="78"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
       <c r="J52" s="20">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="K52" s="18"/>
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
       <c r="N52" s="16">
-        <f t="shared" si="80"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="O52" s="165"/>
       <c r="P52" s="166"/>
       <c r="Q52" s="166"/>
       <c r="R52" s="178">
-        <f t="shared" si="81"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="S52" s="12">
-        <f t="shared" si="83"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
     </row>
@@ -4663,28 +4630,28 @@
       <c r="D53" s="113"/>
       <c r="E53" s="113"/>
       <c r="F53" s="110">
-        <f t="shared" si="78"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="G53" s="22"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
       <c r="J53" s="20">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="K53" s="18"/>
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
       <c r="N53" s="16">
-        <f t="shared" si="80"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="O53" s="165"/>
       <c r="P53" s="166"/>
       <c r="Q53" s="166"/>
       <c r="R53" s="178">
-        <f t="shared" si="81"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="S53" s="12">
@@ -4700,32 +4667,32 @@
       <c r="D54" s="113"/>
       <c r="E54" s="113"/>
       <c r="F54" s="110">
-        <f t="shared" si="78"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="G54" s="22"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="J54" s="20">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="K54" s="18"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
       <c r="N54" s="16">
-        <f t="shared" si="80"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="O54" s="165"/>
       <c r="P54" s="166"/>
       <c r="Q54" s="166"/>
       <c r="R54" s="178">
-        <f t="shared" si="81"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="S54" s="12">
-        <f t="shared" ref="S54" si="84">SUM(F54,J54,N54,R54)</f>
+        <f t="shared" ref="S54" si="81">SUM(F54,J54,N54,R54)</f>
         <v>0</v>
       </c>
     </row>
@@ -4737,28 +4704,28 @@
       <c r="D55" s="113"/>
       <c r="E55" s="113"/>
       <c r="F55" s="110">
-        <f t="shared" si="78"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="G55" s="22"/>
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
       <c r="J55" s="20">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="K55" s="18"/>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
       <c r="N55" s="16">
-        <f t="shared" si="80"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="O55" s="165"/>
       <c r="P55" s="166"/>
       <c r="Q55" s="166"/>
       <c r="R55" s="178">
-        <f t="shared" si="81"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="S55" s="12">
@@ -4774,32 +4741,32 @@
       <c r="D56" s="113"/>
       <c r="E56" s="113"/>
       <c r="F56" s="110">
-        <f t="shared" si="78"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="8"/>
       <c r="I56" s="8"/>
       <c r="J56" s="20">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="K56" s="18"/>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
       <c r="N56" s="16">
-        <f t="shared" si="80"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="O56" s="165"/>
       <c r="P56" s="166"/>
       <c r="Q56" s="166"/>
       <c r="R56" s="178">
-        <f t="shared" si="81"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="S56" s="12">
-        <f t="shared" ref="S56" si="85">SUM(F56,J56,N56,R56)</f>
+        <f t="shared" ref="S56" si="82">SUM(F56,J56,N56,R56)</f>
         <v>0</v>
       </c>
     </row>
@@ -4811,28 +4778,28 @@
       <c r="D57" s="113"/>
       <c r="E57" s="113"/>
       <c r="F57" s="110">
-        <f t="shared" si="78"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
       <c r="J57" s="20">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="K57" s="18"/>
       <c r="L57" s="9"/>
       <c r="M57" s="9"/>
       <c r="N57" s="16">
-        <f t="shared" si="80"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="O57" s="165"/>
       <c r="P57" s="166"/>
       <c r="Q57" s="166"/>
       <c r="R57" s="178">
-        <f t="shared" si="81"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="S57" s="12">
@@ -4853,11 +4820,11 @@
         <v>0</v>
       </c>
       <c r="E58" s="111">
-        <f t="shared" ref="E58" si="86">SUM(E48:E57)</f>
+        <f t="shared" ref="E58" si="83">SUM(E48:E57)</f>
         <v>0</v>
       </c>
       <c r="F58" s="110">
-        <f t="shared" si="78"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="G58" s="23">
@@ -4869,11 +4836,11 @@
         <v>0</v>
       </c>
       <c r="I58" s="24">
-        <f t="shared" ref="I58" si="87">SUM(I48:I57)</f>
+        <f t="shared" ref="I58" si="84">SUM(I48:I57)</f>
         <v>0</v>
       </c>
       <c r="J58" s="20">
-        <f t="shared" si="79"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="K58" s="25">
@@ -4885,11 +4852,11 @@
         <v>0</v>
       </c>
       <c r="M58" s="26">
-        <f t="shared" ref="M58" si="88">SUM(M48:M57)</f>
+        <f t="shared" ref="M58" si="85">SUM(M48:M57)</f>
         <v>0</v>
       </c>
       <c r="N58" s="16">
-        <f t="shared" si="80"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="O58" s="180">
@@ -4905,7 +4872,7 @@
         <v>0</v>
       </c>
       <c r="R58" s="178">
-        <f t="shared" si="81"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="S58" s="38">
@@ -4943,28 +4910,28 @@
       <c r="D60" s="113"/>
       <c r="E60" s="113"/>
       <c r="F60" s="110">
-        <f t="shared" ref="F60:F65" si="89">SUM(C60:E60)</f>
+        <f t="shared" ref="F60:F65" si="86">SUM(C60:E60)</f>
         <v>0</v>
       </c>
       <c r="G60" s="22"/>
       <c r="H60" s="8"/>
       <c r="I60" s="8"/>
       <c r="J60" s="20">
-        <f t="shared" ref="J60:J65" si="90">SUM(G60:I60)</f>
+        <f t="shared" ref="J60:J65" si="87">SUM(G60:I60)</f>
         <v>0</v>
       </c>
       <c r="K60" s="18"/>
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
       <c r="N60" s="16">
-        <f t="shared" ref="N60:N65" si="91">SUM(K60:M60)</f>
+        <f t="shared" ref="N60:N65" si="88">SUM(K60:M60)</f>
         <v>0</v>
       </c>
       <c r="O60" s="165"/>
       <c r="P60" s="166"/>
       <c r="Q60" s="166"/>
       <c r="R60" s="178">
-        <f t="shared" ref="R60:R65" si="92">SUM(O60:Q60)</f>
+        <f t="shared" ref="R60:R65" si="89">SUM(O60:Q60)</f>
         <v>0</v>
       </c>
       <c r="S60" s="12">
@@ -4980,32 +4947,32 @@
       <c r="D61" s="113"/>
       <c r="E61" s="113"/>
       <c r="F61" s="110">
-        <f t="shared" si="89"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="8"/>
       <c r="I61" s="8"/>
       <c r="J61" s="20">
-        <f t="shared" si="90"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="K61" s="18"/>
       <c r="L61" s="9"/>
       <c r="M61" s="9"/>
       <c r="N61" s="16">
-        <f t="shared" si="91"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="O61" s="165"/>
       <c r="P61" s="166"/>
       <c r="Q61" s="166"/>
       <c r="R61" s="178">
-        <f t="shared" si="92"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="S61" s="12">
-        <f t="shared" ref="S61" si="93">SUM(F61,J61,N61,R61)</f>
+        <f t="shared" ref="S61" si="90">SUM(F61,J61,N61,R61)</f>
         <v>0</v>
       </c>
     </row>
@@ -5017,28 +4984,28 @@
       <c r="D62" s="113"/>
       <c r="E62" s="113"/>
       <c r="F62" s="110">
-        <f t="shared" si="89"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="G62" s="22"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
       <c r="J62" s="20">
-        <f t="shared" si="90"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="K62" s="18"/>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
       <c r="N62" s="16">
-        <f t="shared" si="91"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="O62" s="165"/>
       <c r="P62" s="166"/>
       <c r="Q62" s="166"/>
       <c r="R62" s="178">
-        <f t="shared" si="92"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="S62" s="12">
@@ -5054,32 +5021,32 @@
       <c r="D63" s="113"/>
       <c r="E63" s="113"/>
       <c r="F63" s="110">
-        <f t="shared" si="89"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="G63" s="22"/>
       <c r="H63" s="8"/>
       <c r="I63" s="8"/>
       <c r="J63" s="20">
-        <f t="shared" si="90"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="K63" s="18"/>
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
       <c r="N63" s="16">
-        <f t="shared" si="91"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="O63" s="165"/>
       <c r="P63" s="166"/>
       <c r="Q63" s="166"/>
       <c r="R63" s="178">
-        <f t="shared" si="92"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="S63" s="12">
-        <f t="shared" ref="S63:S64" si="94">SUM(F63,J63,N63,R63)</f>
+        <f t="shared" ref="S63:S64" si="91">SUM(F63,J63,N63,R63)</f>
         <v>0</v>
       </c>
     </row>
@@ -5091,32 +5058,32 @@
       <c r="D64" s="113"/>
       <c r="E64" s="113"/>
       <c r="F64" s="110">
-        <f t="shared" si="89"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="G64" s="22"/>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
       <c r="J64" s="20">
-        <f t="shared" si="90"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="K64" s="18"/>
       <c r="L64" s="9"/>
       <c r="M64" s="9"/>
       <c r="N64" s="16">
-        <f t="shared" si="91"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="O64" s="165"/>
       <c r="P64" s="166"/>
       <c r="Q64" s="166"/>
       <c r="R64" s="178">
-        <f t="shared" si="92"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="S64" s="12">
-        <f t="shared" si="94"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
     </row>
@@ -5137,7 +5104,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="110">
-        <f t="shared" si="89"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="G65" s="23">
@@ -5153,7 +5120,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="20">
-        <f t="shared" si="90"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="K65" s="25">
@@ -5169,7 +5136,7 @@
         <v>0</v>
       </c>
       <c r="N65" s="16">
-        <f t="shared" si="91"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="O65" s="180">
@@ -5185,7 +5152,7 @@
         <v>0</v>
       </c>
       <c r="R65" s="178">
-        <f t="shared" si="92"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="S65" s="38">
@@ -5223,28 +5190,28 @@
       <c r="D67" s="113"/>
       <c r="E67" s="113"/>
       <c r="F67" s="110">
-        <f t="shared" ref="F67:F72" si="95">SUM(C67:E67)</f>
+        <f t="shared" ref="F67:F72" si="92">SUM(C67:E67)</f>
         <v>0</v>
       </c>
       <c r="G67" s="22"/>
       <c r="H67" s="8"/>
       <c r="I67" s="8"/>
       <c r="J67" s="20">
-        <f t="shared" ref="J67:J72" si="96">SUM(G67:I67)</f>
+        <f t="shared" ref="J67:J72" si="93">SUM(G67:I67)</f>
         <v>0</v>
       </c>
       <c r="K67" s="18"/>
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
       <c r="N67" s="16">
-        <f t="shared" ref="N67:N72" si="97">SUM(K67:M67)</f>
+        <f t="shared" ref="N67:N72" si="94">SUM(K67:M67)</f>
         <v>0</v>
       </c>
       <c r="O67" s="165"/>
       <c r="P67" s="166"/>
       <c r="Q67" s="166"/>
       <c r="R67" s="178">
-        <f t="shared" ref="R67:R72" si="98">SUM(O67:Q67)</f>
+        <f t="shared" ref="R67:R72" si="95">SUM(O67:Q67)</f>
         <v>0</v>
       </c>
       <c r="S67" s="12">
@@ -5260,32 +5227,32 @@
       <c r="D68" s="113"/>
       <c r="E68" s="113"/>
       <c r="F68" s="110">
-        <f t="shared" si="95"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="G68" s="22"/>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
       <c r="J68" s="20">
-        <f t="shared" si="96"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="K68" s="18"/>
       <c r="L68" s="9"/>
       <c r="M68" s="9"/>
       <c r="N68" s="16">
-        <f t="shared" si="97"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="O68" s="165"/>
       <c r="P68" s="166"/>
       <c r="Q68" s="166"/>
       <c r="R68" s="178">
-        <f t="shared" si="98"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="S68" s="12">
-        <f t="shared" ref="S68" si="99">SUM(F68,J68,N68,R68)</f>
+        <f t="shared" ref="S68" si="96">SUM(F68,J68,N68,R68)</f>
         <v>0</v>
       </c>
     </row>
@@ -5297,28 +5264,28 @@
       <c r="D69" s="113"/>
       <c r="E69" s="113"/>
       <c r="F69" s="110">
-        <f t="shared" si="95"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="G69" s="22"/>
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
       <c r="J69" s="20">
-        <f t="shared" si="96"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="K69" s="18"/>
       <c r="L69" s="9"/>
       <c r="M69" s="9"/>
       <c r="N69" s="16">
-        <f t="shared" si="97"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="O69" s="165"/>
       <c r="P69" s="166"/>
       <c r="Q69" s="166"/>
       <c r="R69" s="178">
-        <f t="shared" si="98"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="S69" s="12">
@@ -5334,32 +5301,32 @@
       <c r="D70" s="113"/>
       <c r="E70" s="113"/>
       <c r="F70" s="110">
-        <f t="shared" si="95"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="G70" s="22"/>
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
       <c r="J70" s="20">
-        <f t="shared" si="96"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="K70" s="18"/>
       <c r="L70" s="9"/>
       <c r="M70" s="9"/>
       <c r="N70" s="16">
-        <f t="shared" si="97"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="O70" s="165"/>
       <c r="P70" s="166"/>
       <c r="Q70" s="166"/>
       <c r="R70" s="178">
-        <f t="shared" si="98"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="S70" s="12">
-        <f t="shared" ref="S70:S71" si="100">SUM(F70,J70,N70,R70)</f>
+        <f t="shared" ref="S70:S71" si="97">SUM(F70,J70,N70,R70)</f>
         <v>0</v>
       </c>
     </row>
@@ -5371,32 +5338,32 @@
       <c r="D71" s="113"/>
       <c r="E71" s="113"/>
       <c r="F71" s="110">
-        <f t="shared" si="95"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="G71" s="22"/>
       <c r="H71" s="8"/>
       <c r="I71" s="8"/>
       <c r="J71" s="20">
-        <f t="shared" si="96"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="K71" s="18"/>
       <c r="L71" s="9"/>
       <c r="M71" s="9"/>
       <c r="N71" s="16">
-        <f t="shared" si="97"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="O71" s="165"/>
       <c r="P71" s="166"/>
       <c r="Q71" s="166"/>
       <c r="R71" s="178">
-        <f t="shared" si="98"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="S71" s="12">
-        <f t="shared" si="100"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
     </row>
@@ -5417,7 +5384,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="110">
-        <f t="shared" si="95"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="G72" s="23">
@@ -5433,7 +5400,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="20">
-        <f t="shared" si="96"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="K72" s="25">
@@ -5449,7 +5416,7 @@
         <v>0</v>
       </c>
       <c r="N72" s="16">
-        <f t="shared" si="97"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="O72" s="180">
@@ -5465,7 +5432,7 @@
         <v>0</v>
       </c>
       <c r="R72" s="178">
-        <f t="shared" si="98"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="S72" s="38">
@@ -5503,28 +5470,28 @@
       <c r="D74" s="113"/>
       <c r="E74" s="113"/>
       <c r="F74" s="110">
-        <f t="shared" ref="F74:F88" si="101">SUM(C74:E74)</f>
+        <f t="shared" ref="F74:F88" si="98">SUM(C74:E74)</f>
         <v>0</v>
       </c>
       <c r="G74" s="22"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
       <c r="J74" s="20">
-        <f t="shared" ref="J74:J88" si="102">SUM(G74:I74)</f>
+        <f t="shared" ref="J74:J88" si="99">SUM(G74:I74)</f>
         <v>0</v>
       </c>
       <c r="K74" s="18"/>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
       <c r="N74" s="16">
-        <f t="shared" ref="N74:N88" si="103">SUM(K74:M74)</f>
+        <f t="shared" ref="N74:N88" si="100">SUM(K74:M74)</f>
         <v>0</v>
       </c>
       <c r="O74" s="165"/>
       <c r="P74" s="166"/>
       <c r="Q74" s="166"/>
       <c r="R74" s="178">
-        <f t="shared" ref="R74:R88" si="104">SUM(O74:Q74)</f>
+        <f t="shared" ref="R74:R88" si="101">SUM(O74:Q74)</f>
         <v>0</v>
       </c>
       <c r="S74" s="12">
@@ -5540,32 +5507,32 @@
       <c r="D75" s="113"/>
       <c r="E75" s="113"/>
       <c r="F75" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G75" s="22"/>
       <c r="H75" s="8"/>
       <c r="I75" s="8"/>
       <c r="J75" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K75" s="18"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
       <c r="N75" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O75" s="165"/>
       <c r="P75" s="166"/>
       <c r="Q75" s="166"/>
       <c r="R75" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S75" s="12">
-        <f t="shared" ref="S75" si="105">SUM(F75,J75,N75,R75)</f>
+        <f t="shared" ref="S75" si="102">SUM(F75,J75,N75,R75)</f>
         <v>0</v>
       </c>
     </row>
@@ -5577,28 +5544,28 @@
       <c r="D76" s="113"/>
       <c r="E76" s="113"/>
       <c r="F76" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G76" s="22"/>
       <c r="H76" s="8"/>
       <c r="I76" s="8"/>
       <c r="J76" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K76" s="18"/>
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
       <c r="N76" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O76" s="165"/>
       <c r="P76" s="166"/>
       <c r="Q76" s="166"/>
       <c r="R76" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S76" s="12">
@@ -5614,32 +5581,32 @@
       <c r="D77" s="113"/>
       <c r="E77" s="113"/>
       <c r="F77" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G77" s="22"/>
       <c r="H77" s="8"/>
       <c r="I77" s="8"/>
       <c r="J77" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K77" s="18"/>
       <c r="L77" s="9"/>
       <c r="M77" s="9"/>
       <c r="N77" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O77" s="165"/>
       <c r="P77" s="166"/>
       <c r="Q77" s="166"/>
       <c r="R77" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S77" s="12">
-        <f t="shared" ref="S77:S78" si="106">SUM(F77,J77,N77,R77)</f>
+        <f t="shared" ref="S77:S78" si="103">SUM(F77,J77,N77,R77)</f>
         <v>0</v>
       </c>
     </row>
@@ -5651,32 +5618,32 @@
       <c r="D78" s="113"/>
       <c r="E78" s="113"/>
       <c r="F78" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G78" s="22"/>
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
       <c r="J78" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K78" s="18"/>
       <c r="L78" s="9"/>
       <c r="M78" s="9"/>
       <c r="N78" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O78" s="165"/>
       <c r="P78" s="166"/>
       <c r="Q78" s="166"/>
       <c r="R78" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S78" s="12">
-        <f t="shared" si="106"/>
+        <f t="shared" si="103"/>
         <v>0</v>
       </c>
     </row>
@@ -5688,28 +5655,28 @@
       <c r="D79" s="113"/>
       <c r="E79" s="113"/>
       <c r="F79" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G79" s="22"/>
       <c r="H79" s="8"/>
       <c r="I79" s="8"/>
       <c r="J79" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K79" s="18"/>
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
       <c r="N79" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O79" s="165"/>
       <c r="P79" s="166"/>
       <c r="Q79" s="166"/>
       <c r="R79" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S79" s="12">
@@ -5725,32 +5692,32 @@
       <c r="D80" s="113"/>
       <c r="E80" s="113"/>
       <c r="F80" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G80" s="22"/>
       <c r="H80" s="8"/>
       <c r="I80" s="8"/>
       <c r="J80" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K80" s="18"/>
       <c r="L80" s="9"/>
       <c r="M80" s="9"/>
       <c r="N80" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O80" s="165"/>
       <c r="P80" s="166"/>
       <c r="Q80" s="166"/>
       <c r="R80" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S80" s="12">
-        <f t="shared" ref="S80" si="107">SUM(F80,J80,N80,R80)</f>
+        <f t="shared" ref="S80" si="104">SUM(F80,J80,N80,R80)</f>
         <v>0</v>
       </c>
     </row>
@@ -5762,28 +5729,28 @@
       <c r="D81" s="113"/>
       <c r="E81" s="113"/>
       <c r="F81" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G81" s="22"/>
       <c r="H81" s="8"/>
       <c r="I81" s="8"/>
       <c r="J81" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K81" s="18"/>
       <c r="L81" s="9"/>
       <c r="M81" s="9"/>
       <c r="N81" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O81" s="165"/>
       <c r="P81" s="166"/>
       <c r="Q81" s="166"/>
       <c r="R81" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S81" s="12">
@@ -5799,28 +5766,28 @@
       <c r="D82" s="113"/>
       <c r="E82" s="113"/>
       <c r="F82" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G82" s="22"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
       <c r="J82" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K82" s="18"/>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
       <c r="N82" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O82" s="165"/>
       <c r="P82" s="166"/>
       <c r="Q82" s="166"/>
       <c r="R82" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S82" s="12">
@@ -5836,32 +5803,32 @@
       <c r="D83" s="113"/>
       <c r="E83" s="113"/>
       <c r="F83" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G83" s="22"/>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
       <c r="J83" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K83" s="18"/>
       <c r="L83" s="9"/>
       <c r="M83" s="9"/>
       <c r="N83" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O83" s="165"/>
       <c r="P83" s="166"/>
       <c r="Q83" s="166"/>
       <c r="R83" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S83" s="12">
-        <f t="shared" ref="S83:S84" si="108">SUM(F83,J83,N83,R83)</f>
+        <f t="shared" ref="S83:S84" si="105">SUM(F83,J83,N83,R83)</f>
         <v>0</v>
       </c>
     </row>
@@ -5873,32 +5840,32 @@
       <c r="D84" s="113"/>
       <c r="E84" s="113"/>
       <c r="F84" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G84" s="22"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
       <c r="J84" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K84" s="18"/>
       <c r="L84" s="9"/>
       <c r="M84" s="9"/>
       <c r="N84" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O84" s="165"/>
       <c r="P84" s="166"/>
       <c r="Q84" s="166"/>
       <c r="R84" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S84" s="12">
-        <f t="shared" si="108"/>
+        <f t="shared" si="105"/>
         <v>0</v>
       </c>
     </row>
@@ -5910,28 +5877,28 @@
       <c r="D85" s="113"/>
       <c r="E85" s="113"/>
       <c r="F85" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G85" s="22"/>
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
       <c r="J85" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K85" s="18"/>
       <c r="L85" s="9"/>
       <c r="M85" s="9"/>
       <c r="N85" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O85" s="165"/>
       <c r="P85" s="166"/>
       <c r="Q85" s="166"/>
       <c r="R85" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S85" s="12">
@@ -5947,32 +5914,32 @@
       <c r="D86" s="113"/>
       <c r="E86" s="113"/>
       <c r="F86" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G86" s="22"/>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
       <c r="J86" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K86" s="18"/>
       <c r="L86" s="9"/>
       <c r="M86" s="9"/>
       <c r="N86" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O86" s="165"/>
       <c r="P86" s="166"/>
       <c r="Q86" s="166"/>
       <c r="R86" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S86" s="12">
-        <f t="shared" ref="S86" si="109">SUM(F86,J86,N86,R86)</f>
+        <f t="shared" ref="S86" si="106">SUM(F86,J86,N86,R86)</f>
         <v>0</v>
       </c>
     </row>
@@ -5984,28 +5951,28 @@
       <c r="D87" s="113"/>
       <c r="E87" s="113"/>
       <c r="F87" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G87" s="22"/>
       <c r="H87" s="8"/>
       <c r="I87" s="8"/>
       <c r="J87" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K87" s="18"/>
       <c r="L87" s="9"/>
       <c r="M87" s="9"/>
       <c r="N87" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O87" s="165"/>
       <c r="P87" s="166"/>
       <c r="Q87" s="166"/>
       <c r="R87" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S87" s="12">
@@ -6030,7 +5997,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="110">
-        <f t="shared" si="101"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="G88" s="23">
@@ -6046,7 +6013,7 @@
         <v>0</v>
       </c>
       <c r="J88" s="20">
-        <f t="shared" si="102"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="K88" s="25">
@@ -6062,7 +6029,7 @@
         <v>0</v>
       </c>
       <c r="N88" s="16">
-        <f t="shared" si="103"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O88" s="180">
@@ -6078,7 +6045,7 @@
         <v>0</v>
       </c>
       <c r="R88" s="178">
-        <f t="shared" si="104"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="S88" s="38">
@@ -6116,28 +6083,28 @@
       <c r="D90" s="113"/>
       <c r="E90" s="113"/>
       <c r="F90" s="110">
-        <f t="shared" ref="F90:F98" si="110">SUM(C90:E90)</f>
+        <f t="shared" ref="F90:F98" si="107">SUM(C90:E90)</f>
         <v>0</v>
       </c>
       <c r="G90" s="22"/>
       <c r="H90" s="8"/>
       <c r="I90" s="8"/>
       <c r="J90" s="20">
-        <f t="shared" ref="J90:J98" si="111">SUM(G90:I90)</f>
+        <f t="shared" ref="J90:J98" si="108">SUM(G90:I90)</f>
         <v>0</v>
       </c>
       <c r="K90" s="18"/>
       <c r="L90" s="9"/>
       <c r="M90" s="9"/>
       <c r="N90" s="16">
-        <f t="shared" ref="N90:N98" si="112">SUM(K90:M90)</f>
+        <f t="shared" ref="N90:N98" si="109">SUM(K90:M90)</f>
         <v>0</v>
       </c>
       <c r="O90" s="165"/>
       <c r="P90" s="166"/>
       <c r="Q90" s="166"/>
       <c r="R90" s="178">
-        <f t="shared" ref="R90:R98" si="113">SUM(O90:Q90)</f>
+        <f t="shared" ref="R90:R98" si="110">SUM(O90:Q90)</f>
         <v>0</v>
       </c>
       <c r="S90" s="12">
@@ -6153,32 +6120,32 @@
       <c r="D91" s="113"/>
       <c r="E91" s="113"/>
       <c r="F91" s="110">
-        <f t="shared" si="110"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="G91" s="22"/>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
       <c r="J91" s="20">
-        <f t="shared" si="111"/>
+        <f t="shared" si="108"/>
         <v>0</v>
       </c>
       <c r="K91" s="18"/>
       <c r="L91" s="9"/>
       <c r="M91" s="9"/>
       <c r="N91" s="16">
-        <f t="shared" si="112"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="O91" s="165"/>
       <c r="P91" s="166"/>
       <c r="Q91" s="166"/>
       <c r="R91" s="178">
-        <f t="shared" si="113"/>
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
       <c r="S91" s="12">
-        <f t="shared" ref="S91" si="114">SUM(F91,J91,N91,R91)</f>
+        <f t="shared" ref="S91" si="111">SUM(F91,J91,N91,R91)</f>
         <v>0</v>
       </c>
     </row>
@@ -6190,28 +6157,28 @@
       <c r="D92" s="113"/>
       <c r="E92" s="113"/>
       <c r="F92" s="110">
-        <f t="shared" si="110"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="G92" s="22"/>
       <c r="H92" s="8"/>
       <c r="I92" s="8"/>
       <c r="J92" s="20">
-        <f t="shared" si="111"/>
+        <f t="shared" si="108"/>
         <v>0</v>
       </c>
       <c r="K92" s="18"/>
       <c r="L92" s="9"/>
       <c r="M92" s="9"/>
       <c r="N92" s="16">
-        <f t="shared" si="112"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="O92" s="165"/>
       <c r="P92" s="166"/>
       <c r="Q92" s="166"/>
       <c r="R92" s="178">
-        <f t="shared" si="113"/>
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
       <c r="S92" s="12">
@@ -6227,32 +6194,32 @@
       <c r="D93" s="113"/>
       <c r="E93" s="113"/>
       <c r="F93" s="110">
-        <f t="shared" si="110"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="G93" s="22"/>
       <c r="H93" s="8"/>
       <c r="I93" s="8"/>
       <c r="J93" s="20">
-        <f t="shared" si="111"/>
+        <f t="shared" si="108"/>
         <v>0</v>
       </c>
       <c r="K93" s="18"/>
       <c r="L93" s="9"/>
       <c r="M93" s="9"/>
       <c r="N93" s="16">
-        <f t="shared" si="112"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="O93" s="165"/>
       <c r="P93" s="166"/>
       <c r="Q93" s="166"/>
       <c r="R93" s="178">
-        <f t="shared" si="113"/>
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
       <c r="S93" s="12">
-        <f t="shared" ref="S93:S94" si="115">SUM(F93,J93,N93,R93)</f>
+        <f t="shared" ref="S93:S94" si="112">SUM(F93,J93,N93,R93)</f>
         <v>0</v>
       </c>
     </row>
@@ -6264,32 +6231,32 @@
       <c r="D94" s="113"/>
       <c r="E94" s="113"/>
       <c r="F94" s="110">
-        <f t="shared" si="110"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="G94" s="22"/>
       <c r="H94" s="8"/>
       <c r="I94" s="8"/>
       <c r="J94" s="20">
-        <f t="shared" si="111"/>
+        <f t="shared" si="108"/>
         <v>0</v>
       </c>
       <c r="K94" s="18"/>
       <c r="L94" s="9"/>
       <c r="M94" s="9"/>
       <c r="N94" s="16">
-        <f t="shared" si="112"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="O94" s="165"/>
       <c r="P94" s="166"/>
       <c r="Q94" s="166"/>
       <c r="R94" s="178">
-        <f t="shared" si="113"/>
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
       <c r="S94" s="12">
-        <f t="shared" si="115"/>
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
     </row>
@@ -6301,28 +6268,28 @@
       <c r="D95" s="113"/>
       <c r="E95" s="113"/>
       <c r="F95" s="110">
-        <f t="shared" si="110"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="G95" s="22"/>
       <c r="H95" s="8"/>
       <c r="I95" s="8"/>
       <c r="J95" s="20">
-        <f t="shared" si="111"/>
+        <f t="shared" si="108"/>
         <v>0</v>
       </c>
       <c r="K95" s="18"/>
       <c r="L95" s="9"/>
       <c r="M95" s="9"/>
       <c r="N95" s="16">
-        <f t="shared" si="112"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="O95" s="165"/>
       <c r="P95" s="166"/>
       <c r="Q95" s="166"/>
       <c r="R95" s="178">
-        <f t="shared" si="113"/>
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
       <c r="S95" s="12">
@@ -6338,32 +6305,32 @@
       <c r="D96" s="113"/>
       <c r="E96" s="113"/>
       <c r="F96" s="110">
-        <f t="shared" si="110"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="G96" s="22"/>
       <c r="H96" s="8"/>
       <c r="I96" s="8"/>
       <c r="J96" s="20">
-        <f t="shared" si="111"/>
+        <f t="shared" si="108"/>
         <v>0</v>
       </c>
       <c r="K96" s="18"/>
       <c r="L96" s="9"/>
       <c r="M96" s="9"/>
       <c r="N96" s="16">
-        <f t="shared" si="112"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="O96" s="165"/>
       <c r="P96" s="166"/>
       <c r="Q96" s="166"/>
       <c r="R96" s="178">
-        <f t="shared" si="113"/>
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
       <c r="S96" s="12">
-        <f t="shared" ref="S96" si="116">SUM(F96,J96,N96,R96)</f>
+        <f t="shared" ref="S96" si="113">SUM(F96,J96,N96,R96)</f>
         <v>0</v>
       </c>
     </row>
@@ -6375,28 +6342,28 @@
       <c r="D97" s="113"/>
       <c r="E97" s="113"/>
       <c r="F97" s="110">
-        <f t="shared" si="110"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="G97" s="22"/>
       <c r="H97" s="8"/>
       <c r="I97" s="8"/>
       <c r="J97" s="20">
-        <f t="shared" si="111"/>
+        <f t="shared" si="108"/>
         <v>0</v>
       </c>
       <c r="K97" s="18"/>
       <c r="L97" s="9"/>
       <c r="M97" s="9"/>
       <c r="N97" s="16">
-        <f t="shared" si="112"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="O97" s="165"/>
       <c r="P97" s="166"/>
       <c r="Q97" s="166"/>
       <c r="R97" s="178">
-        <f t="shared" si="113"/>
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
       <c r="S97" s="12">
@@ -6417,11 +6384,11 @@
         <v>0</v>
       </c>
       <c r="E98" s="111">
-        <f t="shared" ref="E98" si="117">SUM(E90:E97)</f>
+        <f t="shared" ref="E98" si="114">SUM(E90:E97)</f>
         <v>0</v>
       </c>
       <c r="F98" s="110">
-        <f t="shared" si="110"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="G98" s="23">
@@ -6433,11 +6400,11 @@
         <v>0</v>
       </c>
       <c r="I98" s="24">
-        <f t="shared" ref="I98" si="118">SUM(I90:I97)</f>
+        <f t="shared" ref="I98" si="115">SUM(I90:I97)</f>
         <v>0</v>
       </c>
       <c r="J98" s="20">
-        <f t="shared" si="111"/>
+        <f t="shared" si="108"/>
         <v>0</v>
       </c>
       <c r="K98" s="25">
@@ -6449,11 +6416,11 @@
         <v>0</v>
       </c>
       <c r="M98" s="26">
-        <f t="shared" ref="M98" si="119">SUM(M90:M97)</f>
+        <f t="shared" ref="M98" si="116">SUM(M90:M97)</f>
         <v>0</v>
       </c>
       <c r="N98" s="16">
-        <f t="shared" si="112"/>
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
       <c r="O98" s="180">
@@ -6469,7 +6436,7 @@
         <v>0</v>
       </c>
       <c r="R98" s="178">
-        <f t="shared" si="113"/>
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
       <c r="S98" s="38">
@@ -6507,28 +6474,28 @@
       <c r="D100" s="113"/>
       <c r="E100" s="113"/>
       <c r="F100" s="110">
-        <f t="shared" ref="F100:F109" si="120">SUM(C100:E100)</f>
+        <f t="shared" ref="F100:F109" si="117">SUM(C100:E100)</f>
         <v>0</v>
       </c>
       <c r="G100" s="22"/>
       <c r="H100" s="8"/>
       <c r="I100" s="8"/>
       <c r="J100" s="20">
-        <f t="shared" ref="J100:J109" si="121">SUM(G100:I100)</f>
+        <f t="shared" ref="J100:J109" si="118">SUM(G100:I100)</f>
         <v>0</v>
       </c>
       <c r="K100" s="18"/>
       <c r="L100" s="9"/>
       <c r="M100" s="9"/>
       <c r="N100" s="16">
-        <f t="shared" ref="N100:N109" si="122">SUM(K100:M100)</f>
+        <f t="shared" ref="N100:N109" si="119">SUM(K100:M100)</f>
         <v>0</v>
       </c>
       <c r="O100" s="165"/>
       <c r="P100" s="166"/>
       <c r="Q100" s="166"/>
       <c r="R100" s="178">
-        <f t="shared" ref="R100:R109" si="123">SUM(O100:Q100)</f>
+        <f t="shared" ref="R100:R109" si="120">SUM(O100:Q100)</f>
         <v>0</v>
       </c>
       <c r="S100" s="12">
@@ -6544,32 +6511,32 @@
       <c r="D101" s="113"/>
       <c r="E101" s="113"/>
       <c r="F101" s="110">
-        <f t="shared" si="120"/>
+        <f t="shared" si="117"/>
         <v>0</v>
       </c>
       <c r="G101" s="22"/>
       <c r="H101" s="8"/>
       <c r="I101" s="8"/>
       <c r="J101" s="20">
-        <f t="shared" si="121"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="K101" s="18"/>
       <c r="L101" s="9"/>
       <c r="M101" s="9"/>
       <c r="N101" s="16">
-        <f t="shared" si="122"/>
+        <f t="shared" si="119"/>
         <v>0</v>
       </c>
       <c r="O101" s="165"/>
       <c r="P101" s="166"/>
       <c r="Q101" s="166"/>
       <c r="R101" s="178">
-        <f t="shared" si="123"/>
+        <f t="shared" si="120"/>
         <v>0</v>
       </c>
       <c r="S101" s="12">
-        <f t="shared" ref="S101" si="124">SUM(F101,J101,N101,R101)</f>
+        <f t="shared" ref="S101" si="121">SUM(F101,J101,N101,R101)</f>
         <v>0</v>
       </c>
     </row>
@@ -6581,28 +6548,28 @@
       <c r="D102" s="113"/>
       <c r="E102" s="113"/>
       <c r="F102" s="110">
-        <f t="shared" si="120"/>
+        <f t="shared" si="117"/>
         <v>0</v>
       </c>
       <c r="G102" s="22"/>
       <c r="H102" s="8"/>
       <c r="I102" s="8"/>
       <c r="J102" s="20">
-        <f t="shared" si="121"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="K102" s="18"/>
       <c r="L102" s="9"/>
       <c r="M102" s="9"/>
       <c r="N102" s="16">
-        <f t="shared" si="122"/>
+        <f t="shared" si="119"/>
         <v>0</v>
       </c>
       <c r="O102" s="165"/>
       <c r="P102" s="166"/>
       <c r="Q102" s="166"/>
       <c r="R102" s="178">
-        <f t="shared" si="123"/>
+        <f t="shared" si="120"/>
         <v>0</v>
       </c>
       <c r="S102" s="12">
@@ -6618,32 +6585,32 @@
       <c r="D103" s="113"/>
       <c r="E103" s="113"/>
       <c r="F103" s="110">
-        <f t="shared" si="120"/>
+        <f t="shared" si="117"/>
         <v>0</v>
       </c>
       <c r="G103" s="22"/>
       <c r="H103" s="8"/>
       <c r="I103" s="8"/>
       <c r="J103" s="20">
-        <f t="shared" si="121"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="K103" s="18"/>
       <c r="L103" s="9"/>
       <c r="M103" s="9"/>
       <c r="N103" s="16">
-        <f t="shared" si="122"/>
+        <f t="shared" si="119"/>
         <v>0</v>
       </c>
       <c r="O103" s="165"/>
       <c r="P103" s="166"/>
       <c r="Q103" s="166"/>
       <c r="R103" s="178">
-        <f t="shared" si="123"/>
+        <f t="shared" si="120"/>
         <v>0</v>
       </c>
       <c r="S103" s="12">
-        <f t="shared" ref="S103:S104" si="125">SUM(F103,J103,N103,R103)</f>
+        <f t="shared" ref="S103:S104" si="122">SUM(F103,J103,N103,R103)</f>
         <v>0</v>
       </c>
     </row>
@@ -6655,32 +6622,32 @@
       <c r="D104" s="113"/>
       <c r="E104" s="113"/>
       <c r="F104" s="110">
-        <f t="shared" si="120"/>
+        <f t="shared" si="117"/>
         <v>0</v>
       </c>
       <c r="G104" s="22"/>
       <c r="H104" s="8"/>
       <c r="I104" s="8"/>
       <c r="J104" s="20">
-        <f t="shared" si="121"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="K104" s="18"/>
       <c r="L104" s="9"/>
       <c r="M104" s="9"/>
       <c r="N104" s="16">
-        <f t="shared" si="122"/>
+        <f t="shared" si="119"/>
         <v>0</v>
       </c>
       <c r="O104" s="165"/>
       <c r="P104" s="166"/>
       <c r="Q104" s="166"/>
       <c r="R104" s="178">
-        <f t="shared" si="123"/>
+        <f t="shared" si="120"/>
         <v>0</v>
       </c>
       <c r="S104" s="12">
-        <f t="shared" si="125"/>
+        <f t="shared" si="122"/>
         <v>0</v>
       </c>
     </row>
@@ -6692,28 +6659,28 @@
       <c r="D105" s="113"/>
       <c r="E105" s="113"/>
       <c r="F105" s="110">
-        <f t="shared" si="120"/>
+        <f t="shared" si="117"/>
         <v>0</v>
       </c>
       <c r="G105" s="22"/>
       <c r="H105" s="8"/>
       <c r="I105" s="8"/>
       <c r="J105" s="20">
-        <f t="shared" si="121"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="K105" s="18"/>
       <c r="L105" s="9"/>
       <c r="M105" s="9"/>
       <c r="N105" s="16">
-        <f t="shared" si="122"/>
+        <f t="shared" si="119"/>
         <v>0</v>
       </c>
       <c r="O105" s="165"/>
       <c r="P105" s="166"/>
       <c r="Q105" s="166"/>
       <c r="R105" s="178">
-        <f t="shared" si="123"/>
+        <f t="shared" si="120"/>
         <v>0</v>
       </c>
       <c r="S105" s="12">
@@ -6729,32 +6696,32 @@
       <c r="D106" s="113"/>
       <c r="E106" s="113"/>
       <c r="F106" s="110">
-        <f t="shared" si="120"/>
+        <f t="shared" si="117"/>
         <v>0</v>
       </c>
       <c r="G106" s="22"/>
       <c r="H106" s="8"/>
       <c r="I106" s="8"/>
       <c r="J106" s="20">
-        <f t="shared" si="121"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="K106" s="18"/>
       <c r="L106" s="9"/>
       <c r="M106" s="9"/>
       <c r="N106" s="16">
-        <f t="shared" si="122"/>
+        <f t="shared" si="119"/>
         <v>0</v>
       </c>
       <c r="O106" s="165"/>
       <c r="P106" s="166"/>
       <c r="Q106" s="166"/>
       <c r="R106" s="178">
-        <f t="shared" si="123"/>
+        <f t="shared" si="120"/>
         <v>0</v>
       </c>
       <c r="S106" s="12">
-        <f t="shared" ref="S106" si="126">SUM(F106,J106,N106,R106)</f>
+        <f t="shared" ref="S106" si="123">SUM(F106,J106,N106,R106)</f>
         <v>0</v>
       </c>
     </row>
@@ -6766,28 +6733,28 @@
       <c r="D107" s="113"/>
       <c r="E107" s="113"/>
       <c r="F107" s="110">
-        <f t="shared" si="120"/>
+        <f t="shared" si="117"/>
         <v>0</v>
       </c>
       <c r="G107" s="22"/>
       <c r="H107" s="8"/>
       <c r="I107" s="8"/>
       <c r="J107" s="20">
-        <f t="shared" si="121"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="K107" s="18"/>
       <c r="L107" s="9"/>
       <c r="M107" s="9"/>
       <c r="N107" s="16">
-        <f t="shared" si="122"/>
+        <f t="shared" si="119"/>
         <v>0</v>
       </c>
       <c r="O107" s="165"/>
       <c r="P107" s="166"/>
       <c r="Q107" s="166"/>
       <c r="R107" s="178">
-        <f t="shared" si="123"/>
+        <f t="shared" si="120"/>
         <v>0</v>
       </c>
       <c r="S107" s="12">
@@ -6808,11 +6775,11 @@
         <v>0</v>
       </c>
       <c r="E108" s="111">
-        <f t="shared" ref="E108" si="127">SUM(E100:E107)</f>
+        <f t="shared" ref="E108" si="124">SUM(E100:E107)</f>
         <v>0</v>
       </c>
       <c r="F108" s="110">
-        <f t="shared" si="120"/>
+        <f t="shared" si="117"/>
         <v>0</v>
       </c>
       <c r="G108" s="23">
@@ -6824,11 +6791,11 @@
         <v>0</v>
       </c>
       <c r="I108" s="24">
-        <f t="shared" ref="I108" si="128">SUM(I100:I107)</f>
+        <f t="shared" ref="I108" si="125">SUM(I100:I107)</f>
         <v>0</v>
       </c>
       <c r="J108" s="20">
-        <f t="shared" si="121"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="K108" s="25">
@@ -6840,11 +6807,11 @@
         <v>0</v>
       </c>
       <c r="M108" s="26">
-        <f t="shared" ref="M108" si="129">SUM(M100:M107)</f>
+        <f t="shared" ref="M108" si="126">SUM(M100:M107)</f>
         <v>0</v>
       </c>
       <c r="N108" s="16">
-        <f t="shared" si="122"/>
+        <f t="shared" si="119"/>
         <v>0</v>
       </c>
       <c r="O108" s="180">
@@ -6860,7 +6827,7 @@
         <v>0</v>
       </c>
       <c r="R108" s="178">
-        <f t="shared" si="123"/>
+        <f t="shared" si="120"/>
         <v>0</v>
       </c>
       <c r="S108" s="38">
@@ -6877,15 +6844,15 @@
         <v>0</v>
       </c>
       <c r="D109" s="115">
-        <f t="shared" ref="D109:E109" si="130">SUM(D46,D58,D65,D72,D88,D98,D108)</f>
+        <f t="shared" ref="D109:E109" si="127">SUM(D46,D58,D65,D72,D88,D98,D108)</f>
         <v>0</v>
       </c>
       <c r="E109" s="115">
-        <f t="shared" si="130"/>
+        <f t="shared" si="127"/>
         <v>0</v>
       </c>
       <c r="F109" s="114">
-        <f t="shared" si="120"/>
+        <f t="shared" si="117"/>
         <v>0</v>
       </c>
       <c r="G109" s="118">
@@ -6893,15 +6860,15 @@
         <v>0</v>
       </c>
       <c r="H109" s="119">
-        <f t="shared" ref="H109" si="131">SUM(H46,H58,H65,H72,H88,H98,H108)</f>
+        <f t="shared" ref="H109" si="128">SUM(H46,H58,H65,H72,H88,H98,H108)</f>
         <v>0</v>
       </c>
       <c r="I109" s="119">
-        <f t="shared" ref="I109" si="132">SUM(I46,I58,I65,I72,I88,I98,I108)</f>
+        <f t="shared" ref="I109" si="129">SUM(I46,I58,I65,I72,I88,I98,I108)</f>
         <v>0</v>
       </c>
       <c r="J109" s="120">
-        <f t="shared" si="121"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="K109" s="132">
@@ -6909,15 +6876,15 @@
         <v>0</v>
       </c>
       <c r="L109" s="133">
-        <f t="shared" ref="L109" si="133">SUM(L46,L58,L65,L72,L88,L98,L108)</f>
+        <f t="shared" ref="L109" si="130">SUM(L46,L58,L65,L72,L88,L98,L108)</f>
         <v>0</v>
       </c>
       <c r="M109" s="133">
-        <f t="shared" ref="M109" si="134">SUM(M46,M58,M65,M72,M88,M98,M108)</f>
+        <f t="shared" ref="M109" si="131">SUM(M46,M58,M65,M72,M88,M98,M108)</f>
         <v>0</v>
       </c>
       <c r="N109" s="151">
-        <f t="shared" si="122"/>
+        <f t="shared" si="119"/>
         <v>0</v>
       </c>
       <c r="O109" s="162">
@@ -6925,15 +6892,15 @@
         <v>0</v>
       </c>
       <c r="P109" s="163">
-        <f t="shared" ref="P109" si="135">SUM(P46,P58,P65,P72,P88,P98,P108)</f>
+        <f t="shared" ref="P109" si="132">SUM(P46,P58,P65,P72,P88,P98,P108)</f>
         <v>0</v>
       </c>
       <c r="Q109" s="163">
-        <f t="shared" ref="Q109" si="136">SUM(Q46,Q58,Q65,Q72,Q88,Q98,Q108)</f>
+        <f t="shared" ref="Q109" si="133">SUM(Q46,Q58,Q65,Q72,Q88,Q98,Q108)</f>
         <v>0</v>
       </c>
       <c r="R109" s="179">
-        <f t="shared" si="123"/>
+        <f t="shared" si="120"/>
         <v>0</v>
       </c>
       <c r="S109" s="182">
@@ -7028,28 +6995,28 @@
       <c r="D113" s="113"/>
       <c r="E113" s="113"/>
       <c r="F113" s="110">
-        <f t="shared" ref="F113:F121" si="137">SUM(C113:E113)</f>
+        <f t="shared" ref="F113:F121" si="134">SUM(C113:E113)</f>
         <v>0</v>
       </c>
       <c r="G113" s="22"/>
       <c r="H113" s="8"/>
       <c r="I113" s="8"/>
       <c r="J113" s="20">
-        <f t="shared" ref="J113:J121" si="138">SUM(G113:I113)</f>
+        <f t="shared" ref="J113:J121" si="135">SUM(G113:I113)</f>
         <v>0</v>
       </c>
       <c r="K113" s="18"/>
       <c r="L113" s="9"/>
       <c r="M113" s="9"/>
       <c r="N113" s="16">
-        <f t="shared" ref="N113:N121" si="139">SUM(K113:M113)</f>
+        <f t="shared" ref="N113:N121" si="136">SUM(K113:M113)</f>
         <v>0</v>
       </c>
       <c r="O113" s="165"/>
       <c r="P113" s="166"/>
       <c r="Q113" s="166"/>
       <c r="R113" s="178">
-        <f t="shared" ref="R113:R121" si="140">SUM(O113:Q113)</f>
+        <f t="shared" ref="R113:R121" si="137">SUM(O113:Q113)</f>
         <v>0</v>
       </c>
       <c r="S113" s="12">
@@ -7065,32 +7032,32 @@
       <c r="D114" s="113"/>
       <c r="E114" s="113"/>
       <c r="F114" s="110">
-        <f t="shared" si="137"/>
+        <f t="shared" si="134"/>
         <v>0</v>
       </c>
       <c r="G114" s="22"/>
       <c r="H114" s="8"/>
       <c r="I114" s="8"/>
       <c r="J114" s="20">
-        <f t="shared" si="138"/>
+        <f t="shared" si="135"/>
         <v>0</v>
       </c>
       <c r="K114" s="18"/>
       <c r="L114" s="9"/>
       <c r="M114" s="9"/>
       <c r="N114" s="16">
-        <f t="shared" si="139"/>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="O114" s="165"/>
       <c r="P114" s="166"/>
       <c r="Q114" s="166"/>
       <c r="R114" s="178">
-        <f t="shared" si="140"/>
+        <f t="shared" si="137"/>
         <v>0</v>
       </c>
       <c r="S114" s="12">
-        <f t="shared" ref="S114" si="141">SUM(F114,J114,N114,R114)</f>
+        <f t="shared" ref="S114" si="138">SUM(F114,J114,N114,R114)</f>
         <v>0</v>
       </c>
     </row>
@@ -7102,28 +7069,28 @@
       <c r="D115" s="113"/>
       <c r="E115" s="113"/>
       <c r="F115" s="110">
-        <f t="shared" si="137"/>
+        <f t="shared" si="134"/>
         <v>0</v>
       </c>
       <c r="G115" s="22"/>
       <c r="H115" s="8"/>
       <c r="I115" s="8"/>
       <c r="J115" s="20">
-        <f t="shared" si="138"/>
+        <f t="shared" si="135"/>
         <v>0</v>
       </c>
       <c r="K115" s="18"/>
       <c r="L115" s="9"/>
       <c r="M115" s="9"/>
       <c r="N115" s="16">
-        <f t="shared" si="139"/>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="O115" s="165"/>
       <c r="P115" s="166"/>
       <c r="Q115" s="166"/>
       <c r="R115" s="178">
-        <f t="shared" si="140"/>
+        <f t="shared" si="137"/>
         <v>0</v>
       </c>
       <c r="S115" s="12">
@@ -7139,32 +7106,32 @@
       <c r="D116" s="113"/>
       <c r="E116" s="113"/>
       <c r="F116" s="110">
-        <f t="shared" si="137"/>
+        <f t="shared" si="134"/>
         <v>0</v>
       </c>
       <c r="G116" s="22"/>
       <c r="H116" s="8"/>
       <c r="I116" s="8"/>
       <c r="J116" s="20">
-        <f t="shared" si="138"/>
+        <f t="shared" si="135"/>
         <v>0</v>
       </c>
       <c r="K116" s="18"/>
       <c r="L116" s="9"/>
       <c r="M116" s="9"/>
       <c r="N116" s="16">
-        <f t="shared" si="139"/>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="O116" s="165"/>
       <c r="P116" s="166"/>
       <c r="Q116" s="166"/>
       <c r="R116" s="178">
-        <f t="shared" si="140"/>
+        <f t="shared" si="137"/>
         <v>0</v>
       </c>
       <c r="S116" s="12">
-        <f t="shared" ref="S116:S117" si="142">SUM(F116,J116,N116,R116)</f>
+        <f t="shared" ref="S116:S117" si="139">SUM(F116,J116,N116,R116)</f>
         <v>0</v>
       </c>
     </row>
@@ -7176,32 +7143,32 @@
       <c r="D117" s="113"/>
       <c r="E117" s="113"/>
       <c r="F117" s="110">
-        <f t="shared" si="137"/>
+        <f t="shared" si="134"/>
         <v>0</v>
       </c>
       <c r="G117" s="22"/>
       <c r="H117" s="8"/>
       <c r="I117" s="8"/>
       <c r="J117" s="20">
-        <f t="shared" si="138"/>
+        <f t="shared" si="135"/>
         <v>0</v>
       </c>
       <c r="K117" s="18"/>
       <c r="L117" s="9"/>
       <c r="M117" s="9"/>
       <c r="N117" s="16">
-        <f t="shared" si="139"/>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="O117" s="165"/>
       <c r="P117" s="166"/>
       <c r="Q117" s="166"/>
       <c r="R117" s="178">
-        <f t="shared" si="140"/>
+        <f t="shared" si="137"/>
         <v>0</v>
       </c>
       <c r="S117" s="12">
-        <f t="shared" si="142"/>
+        <f t="shared" si="139"/>
         <v>0</v>
       </c>
     </row>
@@ -7213,28 +7180,28 @@
       <c r="D118" s="113"/>
       <c r="E118" s="113"/>
       <c r="F118" s="110">
-        <f t="shared" si="137"/>
+        <f t="shared" si="134"/>
         <v>0</v>
       </c>
       <c r="G118" s="22"/>
       <c r="H118" s="8"/>
       <c r="I118" s="8"/>
       <c r="J118" s="20">
-        <f t="shared" si="138"/>
+        <f t="shared" si="135"/>
         <v>0</v>
       </c>
       <c r="K118" s="18"/>
       <c r="L118" s="9"/>
       <c r="M118" s="9"/>
       <c r="N118" s="16">
-        <f t="shared" si="139"/>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="O118" s="165"/>
       <c r="P118" s="166"/>
       <c r="Q118" s="166"/>
       <c r="R118" s="178">
-        <f t="shared" si="140"/>
+        <f t="shared" si="137"/>
         <v>0</v>
       </c>
       <c r="S118" s="12">
@@ -7250,32 +7217,32 @@
       <c r="D119" s="113"/>
       <c r="E119" s="113"/>
       <c r="F119" s="110">
-        <f t="shared" si="137"/>
+        <f t="shared" si="134"/>
         <v>0</v>
       </c>
       <c r="G119" s="22"/>
       <c r="H119" s="8"/>
       <c r="I119" s="8"/>
       <c r="J119" s="20">
-        <f t="shared" si="138"/>
+        <f t="shared" si="135"/>
         <v>0</v>
       </c>
       <c r="K119" s="18"/>
       <c r="L119" s="9"/>
       <c r="M119" s="9"/>
       <c r="N119" s="16">
-        <f t="shared" si="139"/>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="O119" s="165"/>
       <c r="P119" s="166"/>
       <c r="Q119" s="166"/>
       <c r="R119" s="178">
-        <f t="shared" si="140"/>
+        <f t="shared" si="137"/>
         <v>0</v>
       </c>
       <c r="S119" s="12">
-        <f t="shared" ref="S119" si="143">SUM(F119,J119,N119,R119)</f>
+        <f t="shared" ref="S119" si="140">SUM(F119,J119,N119,R119)</f>
         <v>0</v>
       </c>
     </row>
@@ -7287,28 +7254,28 @@
       <c r="D120" s="113"/>
       <c r="E120" s="113"/>
       <c r="F120" s="110">
-        <f t="shared" si="137"/>
+        <f t="shared" si="134"/>
         <v>0</v>
       </c>
       <c r="G120" s="22"/>
       <c r="H120" s="8"/>
       <c r="I120" s="8"/>
       <c r="J120" s="20">
-        <f t="shared" si="138"/>
+        <f t="shared" si="135"/>
         <v>0</v>
       </c>
       <c r="K120" s="18"/>
       <c r="L120" s="9"/>
       <c r="M120" s="9"/>
       <c r="N120" s="16">
-        <f t="shared" si="139"/>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="O120" s="165"/>
       <c r="P120" s="166"/>
       <c r="Q120" s="166"/>
       <c r="R120" s="178">
-        <f t="shared" si="140"/>
+        <f t="shared" si="137"/>
         <v>0</v>
       </c>
       <c r="S120" s="12">
@@ -7329,11 +7296,11 @@
         <v>0</v>
       </c>
       <c r="E121" s="111">
-        <f t="shared" ref="E121" si="144">SUM(E113:E120)</f>
+        <f t="shared" ref="E121" si="141">SUM(E113:E120)</f>
         <v>0</v>
       </c>
       <c r="F121" s="110">
-        <f t="shared" si="137"/>
+        <f t="shared" si="134"/>
         <v>0</v>
       </c>
       <c r="G121" s="23">
@@ -7345,11 +7312,11 @@
         <v>0</v>
       </c>
       <c r="I121" s="24">
-        <f t="shared" ref="I121" si="145">SUM(I113:I120)</f>
+        <f t="shared" ref="I121" si="142">SUM(I113:I120)</f>
         <v>0</v>
       </c>
       <c r="J121" s="20">
-        <f t="shared" si="138"/>
+        <f t="shared" si="135"/>
         <v>0</v>
       </c>
       <c r="K121" s="25">
@@ -7361,11 +7328,11 @@
         <v>0</v>
       </c>
       <c r="M121" s="26">
-        <f t="shared" ref="M121" si="146">SUM(M113:M120)</f>
+        <f t="shared" ref="M121" si="143">SUM(M113:M120)</f>
         <v>0</v>
       </c>
       <c r="N121" s="16">
-        <f t="shared" si="139"/>
+        <f t="shared" si="136"/>
         <v>0</v>
       </c>
       <c r="O121" s="180">
@@ -7381,7 +7348,7 @@
         <v>0</v>
       </c>
       <c r="R121" s="178">
-        <f t="shared" si="140"/>
+        <f t="shared" si="137"/>
         <v>0</v>
       </c>
       <c r="S121" s="38">
@@ -7419,28 +7386,28 @@
       <c r="D123" s="113"/>
       <c r="E123" s="113"/>
       <c r="F123" s="110">
-        <f t="shared" ref="F123:F133" si="147">SUM(C123:E123)</f>
+        <f t="shared" ref="F123:F133" si="144">SUM(C123:E123)</f>
         <v>0</v>
       </c>
       <c r="G123" s="22"/>
       <c r="H123" s="8"/>
       <c r="I123" s="8"/>
       <c r="J123" s="20">
-        <f t="shared" ref="J123:J133" si="148">SUM(G123:I123)</f>
+        <f t="shared" ref="J123:J133" si="145">SUM(G123:I123)</f>
         <v>0</v>
       </c>
       <c r="K123" s="18"/>
       <c r="L123" s="9"/>
       <c r="M123" s="9"/>
       <c r="N123" s="16">
-        <f t="shared" ref="N123:N133" si="149">SUM(K123:M123)</f>
+        <f t="shared" ref="N123:N133" si="146">SUM(K123:M123)</f>
         <v>0</v>
       </c>
       <c r="O123" s="165"/>
       <c r="P123" s="166"/>
       <c r="Q123" s="166"/>
       <c r="R123" s="178">
-        <f t="shared" ref="R123:R133" si="150">SUM(O123:Q123)</f>
+        <f t="shared" ref="R123:R133" si="147">SUM(O123:Q123)</f>
         <v>0</v>
       </c>
       <c r="S123" s="12">
@@ -7456,32 +7423,32 @@
       <c r="D124" s="113"/>
       <c r="E124" s="113"/>
       <c r="F124" s="110">
-        <f t="shared" si="147"/>
+        <f t="shared" si="144"/>
         <v>0</v>
       </c>
       <c r="G124" s="22"/>
       <c r="H124" s="8"/>
       <c r="I124" s="8"/>
       <c r="J124" s="20">
-        <f t="shared" si="148"/>
+        <f t="shared" si="145"/>
         <v>0</v>
       </c>
       <c r="K124" s="18"/>
       <c r="L124" s="9"/>
       <c r="M124" s="9"/>
       <c r="N124" s="16">
-        <f t="shared" si="149"/>
+        <f t="shared" si="146"/>
         <v>0</v>
       </c>
       <c r="O124" s="165"/>
       <c r="P124" s="166"/>
       <c r="Q124" s="166"/>
       <c r="R124" s="178">
-        <f t="shared" si="150"/>
+        <f t="shared" si="147"/>
         <v>0</v>
       </c>
       <c r="S124" s="12">
-        <f t="shared" ref="S124" si="151">SUM(F124,J124,N124,R124)</f>
+        <f t="shared" ref="S124" si="148">SUM(F124,J124,N124,R124)</f>
         <v>0</v>
       </c>
     </row>
@@ -7493,28 +7460,28 @@
       <c r="D125" s="113"/>
       <c r="E125" s="113"/>
       <c r="F125" s="110">
-        <f t="shared" si="147"/>
+        <f t="shared" si="144"/>
         <v>0</v>
       </c>
       <c r="G125" s="22"/>
       <c r="H125" s="8"/>
       <c r="I125" s="8"/>
       <c r="J125" s="20">
-        <f t="shared" si="148"/>
+        <f t="shared" si="145"/>
         <v>0</v>
       </c>
       <c r="K125" s="18"/>
       <c r="L125" s="9"/>
       <c r="M125" s="9"/>
       <c r="N125" s="16">
-        <f t="shared" si="149"/>
+        <f t="shared" si="146"/>
         <v>0</v>
       </c>
       <c r="O125" s="165"/>
       <c r="P125" s="166"/>
       <c r="Q125" s="166"/>
       <c r="R125" s="178">
-        <f t="shared" si="150"/>
+        <f t="shared" si="147"/>
         <v>0</v>
       </c>
       <c r="S125" s="12">
@@ -7530,32 +7497,32 @@
       <c r="D126" s="113"/>
       <c r="E126" s="113"/>
       <c r="F126" s="110">
-        <f t="shared" si="147"/>
+        <f t="shared" si="144"/>
         <v>0</v>
       </c>
       <c r="G126" s="22"/>
       <c r="H126" s="8"/>
       <c r="I126" s="8"/>
       <c r="J126" s="20">
-        <f t="shared" si="148"/>
+        <f t="shared" si="145"/>
         <v>0</v>
       </c>
       <c r="K126" s="18"/>
       <c r="L126" s="9"/>
       <c r="M126" s="9"/>
       <c r="N126" s="16">
-        <f t="shared" si="149"/>
+        <f t="shared" si="146"/>
         <v>0</v>
       </c>
       <c r="O126" s="165"/>
       <c r="P126" s="166"/>
       <c r="Q126" s="166"/>
       <c r="R126" s="178">
-        <f t="shared" si="150"/>
+        <f t="shared" si="147"/>
         <v>0</v>
       </c>
       <c r="S126" s="12">
-        <f t="shared" ref="S126:S127" si="152">SUM(F126,J126,N126,R126)</f>
+        <f t="shared" ref="S126:S127" si="149">SUM(F126,J126,N126,R126)</f>
         <v>0</v>
       </c>
     </row>
@@ -7567,32 +7534,32 @@
       <c r="D127" s="113"/>
       <c r="E127" s="113"/>
       <c r="F127" s="110">
-        <f t="shared" si="147"/>
+        <f t="shared" si="144"/>
         <v>0</v>
       </c>
       <c r="G127" s="22"/>
       <c r="H127" s="8"/>
       <c r="I127" s="8"/>
       <c r="J127" s="20">
-        <f t="shared" si="148"/>
+        <f t="shared" si="145"/>
         <v>0</v>
       </c>
       <c r="K127" s="18"/>
       <c r="L127" s="9"/>
       <c r="M127" s="9"/>
       <c r="N127" s="16">
-        <f t="shared" si="149"/>
+        <f t="shared" si="146"/>
         <v>0</v>
       </c>
       <c r="O127" s="165"/>
       <c r="P127" s="166"/>
       <c r="Q127" s="166"/>
       <c r="R127" s="178">
-        <f t="shared" si="150"/>
+        <f t="shared" si="147"/>
         <v>0</v>
       </c>
       <c r="S127" s="12">
-        <f t="shared" si="152"/>
+        <f t="shared" si="149"/>
         <v>0</v>
       </c>
     </row>
@@ -7604,28 +7571,28 @@
       <c r="D128" s="113"/>
       <c r="E128" s="113"/>
       <c r="F128" s="110">
-        <f t="shared" si="147"/>
+        <f t="shared" si="144"/>
         <v>0</v>
       </c>
       <c r="G128" s="22"/>
       <c r="H128" s="8"/>
       <c r="I128" s="8"/>
       <c r="J128" s="20">
-        <f t="shared" si="148"/>
+        <f t="shared" si="145"/>
         <v>0</v>
       </c>
       <c r="K128" s="18"/>
       <c r="L128" s="9"/>
       <c r="M128" s="9"/>
       <c r="N128" s="16">
-        <f t="shared" si="149"/>
+        <f t="shared" si="146"/>
         <v>0</v>
       </c>
       <c r="O128" s="165"/>
       <c r="P128" s="166"/>
       <c r="Q128" s="166"/>
       <c r="R128" s="178">
-        <f t="shared" si="150"/>
+        <f t="shared" si="147"/>
         <v>0</v>
       </c>
       <c r="S128" s="12">
@@ -7641,32 +7608,32 @@
       <c r="D129" s="113"/>
       <c r="E129" s="113"/>
       <c r="F129" s="110">
-        <f t="shared" si="147"/>
+        <f t="shared" si="144"/>
         <v>0</v>
       </c>
       <c r="G129" s="22"/>
       <c r="H129" s="8"/>
       <c r="I129" s="8"/>
       <c r="J129" s="20">
-        <f t="shared" si="148"/>
+        <f t="shared" si="145"/>
         <v>0</v>
       </c>
       <c r="K129" s="18"/>
       <c r="L129" s="9"/>
       <c r="M129" s="9"/>
       <c r="N129" s="16">
-        <f t="shared" si="149"/>
+        <f t="shared" si="146"/>
         <v>0</v>
       </c>
       <c r="O129" s="165"/>
       <c r="P129" s="166"/>
       <c r="Q129" s="166"/>
       <c r="R129" s="178">
-        <f t="shared" si="150"/>
+        <f t="shared" si="147"/>
         <v>0</v>
       </c>
       <c r="S129" s="12">
-        <f t="shared" ref="S129" si="153">SUM(F129,J129,N129,R129)</f>
+        <f t="shared" ref="S129" si="150">SUM(F129,J129,N129,R129)</f>
         <v>0</v>
       </c>
     </row>
@@ -7678,28 +7645,28 @@
       <c r="D130" s="113"/>
       <c r="E130" s="113"/>
       <c r="F130" s="110">
-        <f t="shared" si="147"/>
+        <f t="shared" si="144"/>
         <v>0</v>
       </c>
       <c r="G130" s="22"/>
       <c r="H130" s="8"/>
       <c r="I130" s="8"/>
       <c r="J130" s="20">
-        <f t="shared" si="148"/>
+        <f t="shared" si="145"/>
         <v>0</v>
       </c>
       <c r="K130" s="18"/>
       <c r="L130" s="9"/>
       <c r="M130" s="9"/>
       <c r="N130" s="16">
-        <f t="shared" si="149"/>
+        <f t="shared" si="146"/>
         <v>0</v>
       </c>
       <c r="O130" s="165"/>
       <c r="P130" s="166"/>
       <c r="Q130" s="166"/>
       <c r="R130" s="178">
-        <f t="shared" si="150"/>
+        <f t="shared" si="147"/>
         <v>0</v>
       </c>
       <c r="S130" s="12">
@@ -7715,32 +7682,32 @@
       <c r="D131" s="113"/>
       <c r="E131" s="113"/>
       <c r="F131" s="110">
-        <f t="shared" si="147"/>
+        <f t="shared" si="144"/>
         <v>0</v>
       </c>
       <c r="G131" s="22"/>
       <c r="H131" s="8"/>
       <c r="I131" s="8"/>
       <c r="J131" s="20">
-        <f t="shared" si="148"/>
+        <f t="shared" si="145"/>
         <v>0</v>
       </c>
       <c r="K131" s="18"/>
       <c r="L131" s="9"/>
       <c r="M131" s="9"/>
       <c r="N131" s="16">
-        <f t="shared" si="149"/>
+        <f t="shared" si="146"/>
         <v>0</v>
       </c>
       <c r="O131" s="165"/>
       <c r="P131" s="166"/>
       <c r="Q131" s="166"/>
       <c r="R131" s="178">
-        <f t="shared" si="150"/>
+        <f t="shared" si="147"/>
         <v>0</v>
       </c>
       <c r="S131" s="12">
-        <f t="shared" ref="S131" si="154">SUM(F131,J131,N131,R131)</f>
+        <f t="shared" ref="S131" si="151">SUM(F131,J131,N131,R131)</f>
         <v>0</v>
       </c>
     </row>
@@ -7761,7 +7728,7 @@
         <v>0</v>
       </c>
       <c r="F132" s="110">
-        <f t="shared" si="147"/>
+        <f t="shared" si="144"/>
         <v>0</v>
       </c>
       <c r="G132" s="23">
@@ -7777,7 +7744,7 @@
         <v>0</v>
       </c>
       <c r="J132" s="20">
-        <f t="shared" si="148"/>
+        <f t="shared" si="145"/>
         <v>0</v>
       </c>
       <c r="K132" s="25">
@@ -7793,7 +7760,7 @@
         <v>0</v>
       </c>
       <c r="N132" s="16">
-        <f t="shared" si="149"/>
+        <f t="shared" si="146"/>
         <v>0</v>
       </c>
       <c r="O132" s="180">
@@ -7809,7 +7776,7 @@
         <v>0</v>
       </c>
       <c r="R132" s="178">
-        <f t="shared" si="150"/>
+        <f t="shared" si="147"/>
         <v>0</v>
       </c>
       <c r="S132" s="38">
@@ -7826,15 +7793,15 @@
         <v>0</v>
       </c>
       <c r="D133" s="115">
-        <f t="shared" ref="D133:E133" si="155">SUM(D121,D132)</f>
+        <f t="shared" ref="D133:E133" si="152">SUM(D121,D132)</f>
         <v>0</v>
       </c>
       <c r="E133" s="115">
-        <f t="shared" si="155"/>
+        <f t="shared" si="152"/>
         <v>0</v>
       </c>
       <c r="F133" s="114">
-        <f t="shared" si="147"/>
+        <f t="shared" si="144"/>
         <v>0</v>
       </c>
       <c r="G133" s="118">
@@ -7842,15 +7809,15 @@
         <v>0</v>
       </c>
       <c r="H133" s="119">
-        <f t="shared" ref="H133" si="156">SUM(H121,H132)</f>
+        <f t="shared" ref="H133" si="153">SUM(H121,H132)</f>
         <v>0</v>
       </c>
       <c r="I133" s="119">
-        <f t="shared" ref="I133" si="157">SUM(I121,I132)</f>
+        <f t="shared" ref="I133" si="154">SUM(I121,I132)</f>
         <v>0</v>
       </c>
       <c r="J133" s="120">
-        <f t="shared" si="148"/>
+        <f t="shared" si="145"/>
         <v>0</v>
       </c>
       <c r="K133" s="132">
@@ -7858,15 +7825,15 @@
         <v>0</v>
       </c>
       <c r="L133" s="133">
-        <f t="shared" ref="L133" si="158">SUM(L121,L132)</f>
+        <f t="shared" ref="L133" si="155">SUM(L121,L132)</f>
         <v>0</v>
       </c>
       <c r="M133" s="133">
-        <f t="shared" ref="M133" si="159">SUM(M121,M132)</f>
+        <f t="shared" ref="M133" si="156">SUM(M121,M132)</f>
         <v>0</v>
       </c>
       <c r="N133" s="151">
-        <f t="shared" si="149"/>
+        <f t="shared" si="146"/>
         <v>0</v>
       </c>
       <c r="O133" s="162">
@@ -7874,7 +7841,7 @@
         <v>0</v>
       </c>
       <c r="P133" s="163">
-        <f t="shared" ref="P133" si="160">SUM(P121,P132)</f>
+        <f t="shared" ref="P133" si="157">SUM(P121,P132)</f>
         <v>0</v>
       </c>
       <c r="Q133" s="163">
@@ -7882,7 +7849,7 @@
         <v>0</v>
       </c>
       <c r="R133" s="164">
-        <f t="shared" si="150"/>
+        <f t="shared" si="147"/>
         <v>0</v>
       </c>
       <c r="S133" s="182">
@@ -7899,7 +7866,7 @@
         <v>0</v>
       </c>
       <c r="D135" s="115">
-        <f t="shared" ref="D135" si="161">SUM(D109,D133)</f>
+        <f t="shared" ref="D135" si="158">SUM(D109,D133)</f>
         <v>0</v>
       </c>
       <c r="E135" s="115">
@@ -7915,7 +7882,7 @@
         <v>0</v>
       </c>
       <c r="H135" s="119">
-        <f t="shared" ref="H135" si="162">SUM(H109,H133)</f>
+        <f t="shared" ref="H135" si="159">SUM(H109,H133)</f>
         <v>0</v>
       </c>
       <c r="I135" s="119">
@@ -7931,7 +7898,7 @@
         <v>0</v>
       </c>
       <c r="L135" s="133">
-        <f t="shared" ref="L135" si="163">SUM(L109,L133)</f>
+        <f t="shared" ref="L135" si="160">SUM(L109,L133)</f>
         <v>0</v>
       </c>
       <c r="M135" s="133">
@@ -7947,7 +7914,7 @@
         <v>0</v>
       </c>
       <c r="P135" s="163">
-        <f t="shared" ref="P135" si="164">SUM(P109,P133)</f>
+        <f t="shared" ref="P135" si="161">SUM(P109,P133)</f>
         <v>0</v>
       </c>
       <c r="Q135" s="163">
@@ -7984,7 +7951,7 @@
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
-  <pageSetup scale="43" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="43" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8996,7 +8963,7 @@
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>